<commit_message>
Add User Route and Model
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3213" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB7638AE-26FD-4095-9ECB-86C4FC456764}"/>
+  <xr:revisionPtr revIDLastSave="3365" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6FB9A7B-1EC8-4269-8D5D-436E972E3A7C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="751">
   <si>
     <t>Date</t>
   </si>
@@ -2186,7 +2186,109 @@
     <t>Install Express, Nodemon, Initialise Backend, add .gitignore</t>
   </si>
   <si>
-    <t>RESTful Tutorial</t>
+    <t>Take a Complete Node/Express/Mongo/TDD Course to be Able to Correctly Build the Backend of the App (Mosh Intro)</t>
+  </si>
+  <si>
+    <t>Node Architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MERN Course - 1 </t>
+  </si>
+  <si>
+    <t>MERN Course - 2</t>
+  </si>
+  <si>
+    <t>MERN Course - 3</t>
+  </si>
+  <si>
+    <t>Node Module System, Event Emitters, HTTP Module</t>
+  </si>
+  <si>
+    <t>MERN Course - 4</t>
+  </si>
+  <si>
+    <t>NPM and RESTful Services with Express, Postman, HTTP Verbs, Joi</t>
+  </si>
+  <si>
+    <t>MERN Course - 4 Cont</t>
+  </si>
+  <si>
+    <t>Continue Validation (Use Joi@13.1.0!!! Breaking Changes in Further Versions)</t>
+  </si>
+  <si>
+    <t>Build User Request Sceleton</t>
+  </si>
+  <si>
+    <t>Build the Sceleton Code for User GET, POST PUT and DELETE Requests</t>
+  </si>
+  <si>
+    <t>10.03.2023</t>
+  </si>
+  <si>
+    <t>MERN Course - 5</t>
+  </si>
+  <si>
+    <t>Restructure App</t>
+  </si>
+  <si>
+    <t>Apply Routes (Index, User)</t>
+  </si>
+  <si>
+    <t>Advanced Express: Middlewares, Pipeline, Debug, ENV, Config</t>
+  </si>
+  <si>
+    <t>11.03.2023</t>
+  </si>
+  <si>
+    <t>MERN Course - 6</t>
+  </si>
+  <si>
+    <t>MongoDB, Mongoose</t>
+  </si>
+  <si>
+    <t>CRUD Users</t>
+  </si>
+  <si>
+    <t>Create Functions for the Basic CRUD Operations for User Schema</t>
+  </si>
+  <si>
+    <t>MERN Course - 7</t>
+  </si>
+  <si>
+    <t>MongoDB, Mongoose Data Validation</t>
+  </si>
+  <si>
+    <t>User Model</t>
+  </si>
+  <si>
+    <t>Create the User Model and Joi Validation</t>
+  </si>
+  <si>
+    <t>Complete User Routes</t>
+  </si>
+  <si>
+    <t>Express Pipeline Paragraph</t>
+  </si>
+  <si>
+    <t>Express Pipeline Explanation and Diagram</t>
+  </si>
+  <si>
+    <t>Complete and Test User Routes with MongoDB Connection (To be Continued...)</t>
+  </si>
+  <si>
+    <t>Complete User Routes Continued</t>
+  </si>
+  <si>
+    <t>Request GET/api/users/, GET/api/users/:id, POST/api/users{body}</t>
+  </si>
+  <si>
+    <t>Request PUT/api/users/id</t>
+  </si>
+  <si>
+    <t>13.03.2023</t>
+  </si>
+  <si>
+    <t>Profile Route</t>
   </si>
 </sst>
 </file>
@@ -2627,11 +2729,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M599"/>
+  <dimension ref="A1:M610"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E333" sqref="E333"/>
+      <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E348" sqref="E348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -9279,7 +9381,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C332" s="4" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="D332" s="2" t="s">
         <v>37</v>
@@ -9287,192 +9389,431 @@
       <c r="E332" s="2">
         <v>45</v>
       </c>
+      <c r="F332" s="1" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A333" s="5"/>
-      <c r="B333" s="13"/>
-      <c r="C333" s="4"/>
-      <c r="D333" s="2"/>
-      <c r="E333" s="2"/>
+      <c r="A333" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="B333" s="13">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="C333" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="D333" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E333" s="2">
+        <v>25</v>
+      </c>
+      <c r="F333" s="1" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A334" s="5"/>
-      <c r="B334" s="13"/>
-      <c r="C334" s="4"/>
-      <c r="D334" s="2"/>
-      <c r="E334" s="2"/>
+      <c r="A334" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="B334" s="13">
+        <v>0.78125</v>
+      </c>
+      <c r="C334" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="D334" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E334" s="2">
+        <v>55</v>
+      </c>
+      <c r="F334" s="1" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A335" s="5"/>
-      <c r="B335" s="13"/>
-      <c r="C335" s="4"/>
-      <c r="D335" s="2"/>
-      <c r="E335" s="2"/>
+      <c r="A335" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="B335" s="13">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="C335" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="D335" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E335" s="2">
+        <v>90</v>
+      </c>
+      <c r="F335" s="1" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A336" s="5"/>
-      <c r="B336" s="13"/>
-      <c r="C336" s="4"/>
-      <c r="D336" s="2"/>
-      <c r="E336" s="2"/>
-    </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A337" s="5"/>
-      <c r="B337" s="13"/>
-      <c r="C337" s="4"/>
-      <c r="D337" s="2"/>
-      <c r="E337" s="2"/>
-    </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A338" s="5"/>
-      <c r="B338" s="13"/>
-      <c r="C338" s="4"/>
-      <c r="D338" s="2"/>
-      <c r="E338" s="2"/>
-    </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A339" s="5"/>
-      <c r="B339" s="13"/>
-      <c r="C339" s="4"/>
-      <c r="D339" s="2"/>
-      <c r="E339" s="2"/>
-    </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A340" s="5"/>
-      <c r="B340" s="13"/>
-      <c r="C340" s="4"/>
-      <c r="D340" s="2"/>
-      <c r="E340" s="2"/>
-    </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A341" s="5"/>
-      <c r="B341" s="13"/>
-      <c r="C341" s="4"/>
-      <c r="D341" s="2"/>
-      <c r="E341" s="2"/>
-    </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A342" s="5"/>
-      <c r="B342" s="13"/>
-      <c r="C342" s="4"/>
-      <c r="D342" s="2"/>
-      <c r="E342" s="2"/>
-    </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A343" s="10"/>
-      <c r="B343" s="10"/>
-      <c r="D343" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E343" s="3">
-        <f>SUM(E2:E342)</f>
-        <v>30505</v>
-      </c>
-    </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A344" s="10"/>
-      <c r="B344" s="10"/>
-      <c r="D344" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E344" s="3">
-        <f>E343 / 60</f>
-        <v>508.41666666666669</v>
-      </c>
-    </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A345" s="10"/>
-      <c r="B345" s="10"/>
-    </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A346" s="10"/>
-      <c r="B346" s="10"/>
-    </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A347" s="10"/>
-      <c r="B347" s="10"/>
-    </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A348" s="10"/>
-      <c r="B348" s="10"/>
-    </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A349" s="10"/>
-      <c r="B349" s="10"/>
-    </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A350" s="10"/>
-      <c r="B350" s="10"/>
-    </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A351" s="10"/>
-      <c r="B351" s="10"/>
-    </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A352" s="10"/>
-      <c r="B352" s="10"/>
-    </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A353" s="10"/>
-      <c r="B353" s="10"/>
-    </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="B336" s="13">
+        <v>0.84375</v>
+      </c>
+      <c r="C336" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D336" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E336" s="2">
+        <v>20</v>
+      </c>
+      <c r="F336" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="B337" s="13">
+        <v>0.85763888888888884</v>
+      </c>
+      <c r="C337" s="4" t="s">
+        <v>726</v>
+      </c>
+      <c r="D337" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E337" s="2">
+        <v>55</v>
+      </c>
+      <c r="F337" s="1" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="B338" s="13">
+        <v>0.92361111111111116</v>
+      </c>
+      <c r="C338" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="D338" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E338" s="2">
+        <v>55</v>
+      </c>
+      <c r="F338" s="1" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="B339" s="13">
+        <v>0.96180555555555547</v>
+      </c>
+      <c r="C339" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="D339" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E339" s="2">
+        <v>60</v>
+      </c>
+      <c r="F339" s="1" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B340" s="13">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C340" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D340" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E340" s="2">
+        <v>75</v>
+      </c>
+      <c r="F340" s="1" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B341" s="13">
+        <v>5.9027777777777783E-2</v>
+      </c>
+      <c r="C341" s="4" t="s">
+        <v>736</v>
+      </c>
+      <c r="D341" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E341" s="2">
+        <v>60</v>
+      </c>
+      <c r="F341" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B342" s="13">
+        <v>0.10069444444444443</v>
+      </c>
+      <c r="C342" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="D342" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E342" s="2">
+        <v>55</v>
+      </c>
+      <c r="F342" s="1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A343" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B343" s="13">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="C343" s="4" t="s">
+        <v>740</v>
+      </c>
+      <c r="D343" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E343" s="2">
+        <v>25</v>
+      </c>
+      <c r="F343" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A344" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B344" s="13">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C344" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="D344" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E344" s="2">
+        <v>35</v>
+      </c>
+      <c r="F344" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A345" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B345" s="13">
+        <v>0.19097222222222221</v>
+      </c>
+      <c r="C345" s="4" t="s">
+        <v>742</v>
+      </c>
+      <c r="D345" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E345" s="2">
+        <v>45</v>
+      </c>
+      <c r="F345" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B346" s="13">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C346" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="D346" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E346" s="2">
+        <v>55</v>
+      </c>
+      <c r="F346" s="1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B347" s="13">
+        <v>0.625</v>
+      </c>
+      <c r="C347" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="D347" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E347" s="2">
+        <v>45</v>
+      </c>
+      <c r="F347" s="1" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="B348" s="13">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="C348" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D348" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E348" s="2"/>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349" s="5"/>
+      <c r="B349" s="13"/>
+      <c r="C349" s="4"/>
+      <c r="D349" s="2"/>
+      <c r="E349" s="2"/>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350" s="5"/>
+      <c r="B350" s="13"/>
+      <c r="C350" s="4"/>
+      <c r="D350" s="2"/>
+      <c r="E350" s="2"/>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351" s="5"/>
+      <c r="B351" s="13"/>
+      <c r="C351" s="4"/>
+      <c r="D351" s="2"/>
+      <c r="E351" s="2"/>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352" s="5"/>
+      <c r="B352" s="13"/>
+      <c r="C352" s="4"/>
+      <c r="D352" s="2"/>
+      <c r="E352" s="2"/>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A353" s="5"/>
+      <c r="B353" s="13"/>
+      <c r="C353" s="4"/>
+      <c r="D353" s="2"/>
+      <c r="E353" s="2"/>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="10"/>
       <c r="B354" s="10"/>
-    </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D354" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E354" s="3">
+        <f>SUM(E2:E353)</f>
+        <v>31260</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="10"/>
       <c r="B355" s="10"/>
-    </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D355" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E355" s="3">
+        <f>E354 / 60</f>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="10"/>
       <c r="B356" s="10"/>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="10"/>
       <c r="B357" s="10"/>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="10"/>
       <c r="B358" s="10"/>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="10"/>
       <c r="B359" s="10"/>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="10"/>
       <c r="B360" s="10"/>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="10"/>
       <c r="B361" s="10"/>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="10"/>
       <c r="B362" s="10"/>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="10"/>
       <c r="B363" s="10"/>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="10"/>
       <c r="B364" s="10"/>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="10"/>
       <c r="B365" s="10"/>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="10"/>
       <c r="B366" s="10"/>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="10"/>
       <c r="B367" s="10"/>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="10"/>
       <c r="B368" s="10"/>
     </row>
@@ -10399,6 +10740,50 @@
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A599" s="10"/>
       <c r="B599" s="10"/>
+    </row>
+    <row r="600" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A600" s="10"/>
+      <c r="B600" s="10"/>
+    </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A601" s="10"/>
+      <c r="B601" s="10"/>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A602" s="10"/>
+      <c r="B602" s="10"/>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A603" s="10"/>
+      <c r="B603" s="10"/>
+    </row>
+    <row r="604" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A604" s="10"/>
+      <c r="B604" s="10"/>
+    </row>
+    <row r="605" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A605" s="10"/>
+      <c r="B605" s="10"/>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A606" s="10"/>
+      <c r="B606" s="10"/>
+    </row>
+    <row r="607" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A607" s="10"/>
+      <c r="B607" s="10"/>
+    </row>
+    <row r="608" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A608" s="10"/>
+      <c r="B608" s="10"/>
+    </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A609" s="10"/>
+      <c r="B609" s="10"/>
+    </row>
+    <row r="610" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A610" s="10"/>
+      <c r="B610" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Profile Router and Model
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3365" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6FB9A7B-1EC8-4269-8D5D-436E972E3A7C}"/>
+  <xr:revisionPtr revIDLastSave="3375" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39FCA281-492D-45D7-A1E9-6BBF69A563E9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="754">
   <si>
     <t>Date</t>
   </si>
@@ -2288,7 +2288,16 @@
     <t>13.03.2023</t>
   </si>
   <si>
-    <t>Profile Route</t>
+    <t>Profile Model</t>
+  </si>
+  <si>
+    <t>Create Profile Model and Validation</t>
+  </si>
+  <si>
+    <t>Profile Router</t>
+  </si>
+  <si>
+    <t>Profile Routes: GET:api/profiles/:ID, POST:/api/profiles/{body}</t>
   </si>
 </sst>
 </file>
@@ -2731,9 +2740,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
   <dimension ref="A1:M610"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E348" sqref="E348"/>
+      <selection pane="bottomLeft" activeCell="F350" sqref="F350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -9706,14 +9715,32 @@
       <c r="D348" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E348" s="2"/>
+      <c r="E348" s="2">
+        <v>90</v>
+      </c>
+      <c r="F348" s="1" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A349" s="5"/>
-      <c r="B349" s="13"/>
-      <c r="C349" s="4"/>
-      <c r="D349" s="2"/>
-      <c r="E349" s="2"/>
+      <c r="A349" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="B349" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C349" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="D349" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E349" s="2">
+        <v>100</v>
+      </c>
+      <c r="F349" s="1" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350" s="5"/>
@@ -9751,7 +9778,7 @@
       </c>
       <c r="E354" s="3">
         <f>SUM(E2:E353)</f>
-        <v>31260</v>
+        <v>31450</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
@@ -9762,7 +9789,7 @@
       </c>
       <c r="E355" s="3">
         <f>E354 / 60</f>
-        <v>521</v>
+        <v>524.16666666666663</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tabs Route and Model
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3375" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39FCA281-492D-45D7-A1E9-6BBF69A563E9}"/>
+  <xr:revisionPtr revIDLastSave="3403" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{743AC2AE-9C0D-41B4-82F3-B181243736B5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="761">
   <si>
     <t>Date</t>
   </si>
@@ -2298,6 +2298,27 @@
   </si>
   <si>
     <t>Profile Routes: GET:api/profiles/:ID, POST:/api/profiles/{body}</t>
+  </si>
+  <si>
+    <t>MERN Course - 8</t>
+  </si>
+  <si>
+    <t>Data Relationship (Normalisation / Denormalisation)</t>
+  </si>
+  <si>
+    <t>Tabs Model</t>
+  </si>
+  <si>
+    <t>Create Tabs Model Schema</t>
+  </si>
+  <si>
+    <t>14.03.2023</t>
+  </si>
+  <si>
+    <t>Tabs Router</t>
+  </si>
+  <si>
+    <t>Tabs Routes: GET:api/tabs, GET:api/tabs/:ID, POST:/api/tabs/:ID{body}, DEL:/api/tabs/:ID</t>
   </si>
 </sst>
 </file>
@@ -2738,11 +2759,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M610"/>
+  <dimension ref="A1:M612"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F350" sqref="F350"/>
+      <selection pane="bottomLeft" activeCell="F351" sqref="F351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -9743,25 +9764,62 @@
       </c>
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A350" s="5"/>
-      <c r="B350" s="13"/>
-      <c r="C350" s="4"/>
-      <c r="D350" s="2"/>
-      <c r="E350" s="2"/>
+      <c r="A350" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="B350" s="13">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C350" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="D350" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E350" s="2">
+        <v>65</v>
+      </c>
+      <c r="F350" s="1" t="s">
+        <v>757</v>
+      </c>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A351" s="5"/>
-      <c r="B351" s="13"/>
-      <c r="C351" s="4"/>
-      <c r="D351" s="2"/>
-      <c r="E351" s="2"/>
+      <c r="A351" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="B351" s="13">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="C351" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="D351" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E351" s="2">
+        <v>120</v>
+      </c>
+      <c r="F351" s="1" t="s">
+        <v>760</v>
+      </c>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A352" s="5"/>
-      <c r="B352" s="13"/>
-      <c r="C352" s="4"/>
-      <c r="D352" s="2"/>
+      <c r="A352" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="B352" s="13">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C352" s="4" t="s">
+        <v>754</v>
+      </c>
+      <c r="D352" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E352" s="2"/>
+      <c r="F352" s="1" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="5"/>
@@ -9771,34 +9829,40 @@
       <c r="E353" s="2"/>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A354" s="10"/>
-      <c r="B354" s="10"/>
-      <c r="D354" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E354" s="3">
-        <f>SUM(E2:E353)</f>
-        <v>31450</v>
-      </c>
+      <c r="A354" s="5"/>
+      <c r="B354" s="13"/>
+      <c r="C354" s="4"/>
+      <c r="D354" s="2"/>
+      <c r="E354" s="2"/>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A355" s="10"/>
-      <c r="B355" s="10"/>
-      <c r="D355" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E355" s="3">
-        <f>E354 / 60</f>
-        <v>524.16666666666663</v>
-      </c>
+      <c r="A355" s="5"/>
+      <c r="B355" s="13"/>
+      <c r="C355" s="4"/>
+      <c r="D355" s="2"/>
+      <c r="E355" s="2"/>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="10"/>
       <c r="B356" s="10"/>
+      <c r="D356" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E356" s="3">
+        <f>SUM(E2:E355)</f>
+        <v>31635</v>
+      </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="10"/>
       <c r="B357" s="10"/>
+      <c r="D357" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E357" s="3">
+        <f>E356 / 60</f>
+        <v>527.25</v>
+      </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="10"/>
@@ -10811,6 +10875,14 @@
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A610" s="10"/>
       <c r="B610" s="10"/>
+    </row>
+    <row r="611" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A611" s="10"/>
+      <c r="B611" s="10"/>
+    </row>
+    <row r="612" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A612" s="10"/>
+      <c r="B612" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Achievements Route and Model
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3403" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{743AC2AE-9C0D-41B4-82F3-B181243736B5}"/>
+  <xr:revisionPtr revIDLastSave="3411" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AC67A83-7D3C-44E9-BBBD-805D5710E449}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="763">
   <si>
     <t>Date</t>
   </si>
@@ -2319,6 +2319,12 @@
   </si>
   <si>
     <t>Tabs Routes: GET:api/tabs, GET:api/tabs/:ID, POST:/api/tabs/:ID{body}, DEL:/api/tabs/:ID</t>
+  </si>
+  <si>
+    <t>Achievements</t>
+  </si>
+  <si>
+    <t>Achievment Routes: GET:/api/achievements/, GET:/api/achievements/:NAME, POST:/api/achievements/{body}, and Rewise Status Response Codes</t>
   </si>
 </sst>
 </file>
@@ -2456,10 +2462,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2759,11 +2761,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M612"/>
+  <dimension ref="A1:M613"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F351" sqref="F351"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A330" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F352" sqref="F352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -9808,103 +9810,119 @@
         <v>758</v>
       </c>
       <c r="B352" s="13">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C352" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="D352" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E352" s="2">
+        <v>70</v>
+      </c>
+      <c r="F352" s="1" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="B353" s="13">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C352" s="4" t="s">
+      <c r="C353" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="D352" s="2" t="s">
+      <c r="D353" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E352" s="2"/>
-      <c r="F352" s="1" t="s">
+      <c r="E353" s="2"/>
+      <c r="F353" s="1" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A353" s="5"/>
-      <c r="B353" s="13"/>
-      <c r="C353" s="4"/>
-      <c r="D353" s="2"/>
-      <c r="E353" s="2"/>
-    </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354" s="5"/>
       <c r="B354" s="13"/>
       <c r="C354" s="4"/>
       <c r="D354" s="2"/>
       <c r="E354" s="2"/>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355" s="5"/>
       <c r="B355" s="13"/>
       <c r="C355" s="4"/>
       <c r="D355" s="2"/>
       <c r="E355" s="2"/>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A356" s="10"/>
-      <c r="B356" s="10"/>
-      <c r="D356" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E356" s="3">
-        <f>SUM(E2:E355)</f>
-        <v>31635</v>
-      </c>
-    </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356" s="5"/>
+      <c r="B356" s="13"/>
+      <c r="C356" s="4"/>
+      <c r="D356" s="2"/>
+      <c r="E356" s="2"/>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357" s="10"/>
       <c r="B357" s="10"/>
       <c r="D357" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E357" s="3">
-        <f>E356 / 60</f>
-        <v>527.25</v>
-      </c>
-    </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+        <f>SUM(E2:E356)</f>
+        <v>31705</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358" s="10"/>
       <c r="B358" s="10"/>
-    </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D358" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E358" s="3">
+        <f>E357 / 60</f>
+        <v>528.41666666666663</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359" s="10"/>
       <c r="B359" s="10"/>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360" s="10"/>
       <c r="B360" s="10"/>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361" s="10"/>
       <c r="B361" s="10"/>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362" s="10"/>
       <c r="B362" s="10"/>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363" s="10"/>
       <c r="B363" s="10"/>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364" s="10"/>
       <c r="B364" s="10"/>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365" s="10"/>
       <c r="B365" s="10"/>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" s="10"/>
       <c r="B366" s="10"/>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367" s="10"/>
       <c r="B367" s="10"/>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" s="10"/>
       <c r="B368" s="10"/>
     </row>
@@ -10883,6 +10901,10 @@
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A612" s="10"/>
       <c r="B612" s="10"/>
+    </row>
+    <row r="613" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A613" s="10"/>
+      <c r="B613" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Refactor API and Validate IDs, Hide Passwords
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3411" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AC67A83-7D3C-44E9-BBBD-805D5710E449}"/>
+  <xr:revisionPtr revIDLastSave="3447" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA0F32A6-CC80-4171-8433-D6A3430DF5DB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="771">
   <si>
     <t>Date</t>
   </si>
@@ -2303,9 +2303,6 @@
     <t>MERN Course - 8</t>
   </si>
   <si>
-    <t>Data Relationship (Normalisation / Denormalisation)</t>
-  </si>
-  <si>
     <t>Tabs Model</t>
   </si>
   <si>
@@ -2325,6 +2322,33 @@
   </si>
   <si>
     <t>Achievment Routes: GET:/api/achievements/, GET:/api/achievements/:NAME, POST:/api/achievements/{body}, and Rewise Status Response Codes</t>
+  </si>
+  <si>
+    <t>Profile-Achievements Relation</t>
+  </si>
+  <si>
+    <t>Save Achievements as an Array of ObjectIDs, and Create Route PUT:/api/profile/:ID {body}</t>
+  </si>
+  <si>
+    <t>Improve Routes and Models</t>
+  </si>
+  <si>
+    <t>Populate, Hide Password, Iterate and Validate PUT ObjectIDs for Subdocuments</t>
+  </si>
+  <si>
+    <t>Data Relationship (Normalisation / Denormalisation), Populate, Transactions, ObjectID Generation</t>
+  </si>
+  <si>
+    <t>15.03.2023</t>
+  </si>
+  <si>
+    <t>MERN Course - 9</t>
+  </si>
+  <si>
+    <t>Authentication and Authorization</t>
+  </si>
+  <si>
+    <t>Create Login and Auth</t>
   </si>
 </sst>
 </file>
@@ -2462,6 +2486,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2761,11 +2789,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M613"/>
+  <dimension ref="A1:M615"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A330" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F352" sqref="F352"/>
+      <selection pane="bottomLeft" activeCell="A357" sqref="A357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -9767,13 +9795,13 @@
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B350" s="13">
         <v>0.58333333333333337</v>
       </c>
       <c r="C350" s="4" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D350" s="2" t="s">
         <v>162</v>
@@ -9782,18 +9810,18 @@
         <v>65</v>
       </c>
       <c r="F350" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B351" s="13">
         <v>0.63194444444444442</v>
       </c>
       <c r="C351" s="4" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D351" s="2" t="s">
         <v>162</v>
@@ -9802,18 +9830,18 @@
         <v>120</v>
       </c>
       <c r="F351" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B352" s="13">
         <v>0.72222222222222221</v>
       </c>
       <c r="C352" s="4" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D352" s="2" t="s">
         <v>162</v>
@@ -9822,77 +9850,128 @@
         <v>70</v>
       </c>
       <c r="F352" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B353" s="13">
-        <v>0.64583333333333337</v>
+        <v>0.88541666666666663</v>
       </c>
       <c r="C353" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="D353" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E353" s="2">
+        <v>70</v>
+      </c>
+      <c r="F353" s="1" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="B354" s="13">
+        <v>0.9375</v>
+      </c>
+      <c r="C354" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="D353" s="2" t="s">
+      <c r="D354" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E353" s="2"/>
-      <c r="F353" s="1" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A354" s="5"/>
-      <c r="B354" s="13"/>
-      <c r="C354" s="4"/>
-      <c r="D354" s="2"/>
-      <c r="E354" s="2"/>
+      <c r="E354" s="2">
+        <v>50</v>
+      </c>
+      <c r="F354" s="1" t="s">
+        <v>766</v>
+      </c>
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A355" s="5"/>
-      <c r="B355" s="13"/>
-      <c r="C355" s="4"/>
-      <c r="D355" s="2"/>
-      <c r="E355" s="2"/>
+      <c r="A355" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="B355" s="13">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="C355" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="D355" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E355" s="2">
+        <v>145</v>
+      </c>
+      <c r="F355" s="1" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="356" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A356" s="5"/>
-      <c r="B356" s="13"/>
-      <c r="C356" s="4"/>
-      <c r="D356" s="2"/>
+      <c r="A356" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="B356" s="13">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="C356" s="4" t="s">
+        <v>768</v>
+      </c>
+      <c r="D356" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E356" s="2"/>
+      <c r="F356" s="1" t="s">
+        <v>769</v>
+      </c>
     </row>
     <row r="357" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A357" s="10"/>
-      <c r="B357" s="10"/>
-      <c r="D357" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E357" s="3">
-        <f>SUM(E2:E356)</f>
-        <v>31705</v>
-      </c>
+      <c r="A357" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="B357" s="13"/>
+      <c r="C357" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="D357" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E357" s="2"/>
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A358" s="10"/>
-      <c r="B358" s="10"/>
-      <c r="D358" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E358" s="3">
-        <f>E357 / 60</f>
-        <v>528.41666666666663</v>
-      </c>
+      <c r="A358" s="5"/>
+      <c r="B358" s="13"/>
+      <c r="C358" s="4"/>
+      <c r="D358" s="2"/>
+      <c r="E358" s="2"/>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359" s="10"/>
       <c r="B359" s="10"/>
+      <c r="D359" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E359" s="3">
+        <f>SUM(E2:E358)</f>
+        <v>31970</v>
+      </c>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360" s="10"/>
       <c r="B360" s="10"/>
+      <c r="D360" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E360" s="3">
+        <f>E359 / 60</f>
+        <v>532.83333333333337</v>
+      </c>
     </row>
     <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361" s="10"/>
@@ -10905,6 +10984,14 @@
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A613" s="10"/>
       <c r="B613" s="10"/>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A614" s="10"/>
+      <c r="B614" s="10"/>
+    </row>
+    <row r="615" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A615" s="10"/>
+      <c r="B615" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Add Autorization and Authentication
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3447" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA0F32A6-CC80-4171-8433-D6A3430DF5DB}"/>
+  <xr:revisionPtr revIDLastSave="3471" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{188FFF9B-617C-4647-B6C2-19B4AE2E17C8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="774">
   <si>
     <t>Date</t>
   </si>
@@ -2349,6 +2349,15 @@
   </si>
   <si>
     <t>Create Login and Auth</t>
+  </si>
+  <si>
+    <t>Security Diagram</t>
+  </si>
+  <si>
+    <t>Discrete Password Forms, Frontend Hashing, HTTPS, Encrypting and Salting, Comparing</t>
+  </si>
+  <si>
+    <t>Hash, Compare and Validate Password, JWT, Authorization, Admin Privilages</t>
   </si>
 </sst>
 </file>
@@ -2789,11 +2798,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M615"/>
+  <dimension ref="A1:M624"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A330" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A357" sqref="A357"/>
+      <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A359" sqref="A359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -9926,7 +9935,9 @@
       <c r="D356" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E356" s="2"/>
+      <c r="E356" s="2">
+        <v>65</v>
+      </c>
       <c r="F356" s="1" t="s">
         <v>769</v>
       </c>
@@ -9935,137 +9946,184 @@
       <c r="A357" s="5" t="s">
         <v>767</v>
       </c>
-      <c r="B357" s="13"/>
+      <c r="B357" s="13">
+        <v>0.11805555555555557</v>
+      </c>
       <c r="C357" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="D357" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E357" s="2">
+        <v>25</v>
+      </c>
+      <c r="F357" s="1" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="B358" s="13">
+        <v>0.6875</v>
+      </c>
+      <c r="C358" s="4" t="s">
         <v>770</v>
       </c>
-      <c r="D357" s="2" t="s">
+      <c r="D358" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E357" s="2"/>
-    </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A358" s="5"/>
-      <c r="B358" s="13"/>
-      <c r="C358" s="4"/>
-      <c r="D358" s="2"/>
-      <c r="E358" s="2"/>
+      <c r="E358" s="2">
+        <v>195</v>
+      </c>
+      <c r="F358" s="1" t="s">
+        <v>773</v>
+      </c>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A359" s="10"/>
-      <c r="B359" s="10"/>
-      <c r="D359" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E359" s="3">
-        <f>SUM(E2:E358)</f>
-        <v>31970</v>
-      </c>
+      <c r="A359" s="5"/>
+      <c r="B359" s="13"/>
+      <c r="C359" s="4"/>
+      <c r="D359" s="2"/>
+      <c r="E359" s="2"/>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A360" s="10"/>
-      <c r="B360" s="10"/>
-      <c r="D360" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E360" s="3">
-        <f>E359 / 60</f>
-        <v>532.83333333333337</v>
-      </c>
+      <c r="A360" s="5"/>
+      <c r="B360" s="13"/>
+      <c r="C360" s="4"/>
+      <c r="D360" s="2"/>
+      <c r="E360" s="2"/>
     </row>
     <row r="361" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A361" s="10"/>
-      <c r="B361" s="10"/>
+      <c r="A361" s="5"/>
+      <c r="B361" s="13"/>
+      <c r="C361" s="4"/>
+      <c r="D361" s="2"/>
+      <c r="E361" s="2"/>
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A362" s="10"/>
-      <c r="B362" s="10"/>
+      <c r="A362" s="5"/>
+      <c r="B362" s="13"/>
+      <c r="C362" s="4"/>
+      <c r="D362" s="2"/>
+      <c r="E362" s="2"/>
     </row>
     <row r="363" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A363" s="10"/>
-      <c r="B363" s="10"/>
+      <c r="A363" s="5"/>
+      <c r="B363" s="13"/>
+      <c r="C363" s="4"/>
+      <c r="D363" s="2"/>
+      <c r="E363" s="2"/>
     </row>
     <row r="364" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A364" s="10"/>
-      <c r="B364" s="10"/>
+      <c r="A364" s="5"/>
+      <c r="B364" s="13"/>
+      <c r="C364" s="4"/>
+      <c r="D364" s="2"/>
+      <c r="E364" s="2"/>
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A365" s="10"/>
-      <c r="B365" s="10"/>
+      <c r="A365" s="5"/>
+      <c r="B365" s="13"/>
+      <c r="C365" s="4"/>
+      <c r="D365" s="2"/>
+      <c r="E365" s="2"/>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A366" s="10"/>
-      <c r="B366" s="10"/>
+      <c r="A366" s="5"/>
+      <c r="B366" s="13"/>
+      <c r="C366" s="4"/>
+      <c r="D366" s="2"/>
+      <c r="E366" s="2"/>
     </row>
     <row r="367" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A367" s="10"/>
-      <c r="B367" s="10"/>
+      <c r="A367" s="5"/>
+      <c r="B367" s="13"/>
+      <c r="C367" s="4"/>
+      <c r="D367" s="2"/>
+      <c r="E367" s="2"/>
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" s="10"/>
       <c r="B368" s="10"/>
-    </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D368" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E368" s="3">
+        <f>SUM(E2:E367)</f>
+        <v>32255</v>
+      </c>
+    </row>
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="10"/>
       <c r="B369" s="10"/>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D369" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E369" s="3">
+        <f>E368 / 60</f>
+        <v>537.58333333333337</v>
+      </c>
+    </row>
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="10"/>
       <c r="B370" s="10"/>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="10"/>
       <c r="B371" s="10"/>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="10"/>
       <c r="B372" s="10"/>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="10"/>
       <c r="B373" s="10"/>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="10"/>
       <c r="B374" s="10"/>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="10"/>
       <c r="B375" s="10"/>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="10"/>
       <c r="B376" s="10"/>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="10"/>
       <c r="B377" s="10"/>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="10"/>
       <c r="B378" s="10"/>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="10"/>
       <c r="B379" s="10"/>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="10"/>
       <c r="B380" s="10"/>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A381" s="10"/>
       <c r="B381" s="10"/>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A382" s="10"/>
       <c r="B382" s="10"/>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A383" s="10"/>
       <c r="B383" s="10"/>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A384" s="10"/>
       <c r="B384" s="10"/>
     </row>
@@ -10992,6 +11050,42 @@
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A615" s="10"/>
       <c r="B615" s="10"/>
+    </row>
+    <row r="616" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A616" s="10"/>
+      <c r="B616" s="10"/>
+    </row>
+    <row r="617" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A617" s="10"/>
+      <c r="B617" s="10"/>
+    </row>
+    <row r="618" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A618" s="10"/>
+      <c r="B618" s="10"/>
+    </row>
+    <row r="619" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A619" s="10"/>
+      <c r="B619" s="10"/>
+    </row>
+    <row r="620" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A620" s="10"/>
+      <c r="B620" s="10"/>
+    </row>
+    <row r="621" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A621" s="10"/>
+      <c r="B621" s="10"/>
+    </row>
+    <row r="622" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A622" s="10"/>
+      <c r="B622" s="10"/>
+    </row>
+    <row r="623" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A623" s="10"/>
+      <c r="B623" s="10"/>
+    </row>
+    <row r="624" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A624" s="10"/>
+      <c r="B624" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Create Login Form and Validate Input
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3471" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{188FFF9B-617C-4647-B6C2-19B4AE2E17C8}"/>
+  <xr:revisionPtr revIDLastSave="3522" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09D7700A-4097-4CAA-9D60-4FE1E3E2050E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="788">
   <si>
     <t>Date</t>
   </si>
@@ -2358,6 +2358,48 @@
   </si>
   <si>
     <t>Hash, Compare and Validate Password, JWT, Authorization, Admin Privilages</t>
+  </si>
+  <si>
+    <t>MERN Course - 10</t>
+  </si>
+  <si>
+    <t>Handling and Logging Errors, Automated Testing and TDD</t>
+  </si>
+  <si>
+    <t>MERN Course - 11</t>
+  </si>
+  <si>
+    <t>Unit Testing</t>
+  </si>
+  <si>
+    <t>Unit Tests</t>
+  </si>
+  <si>
+    <t>Build Unit Tests</t>
+  </si>
+  <si>
+    <t>MERN Course - 12</t>
+  </si>
+  <si>
+    <t>Integration Testing and TDD</t>
+  </si>
+  <si>
+    <t>Create Login Page</t>
+  </si>
+  <si>
+    <t>Redirect to Login Page When No User Token Found</t>
+  </si>
+  <si>
+    <t>16.03.2023</t>
+  </si>
+  <si>
+    <t>Login Validation</t>
+  </si>
+  <si>
+    <t>Validate Edge Cases on Both Email and Password Inputs and Display User Message</t>
+  </si>
+  <si>
+    <t>Send POST:/api/login</t>
   </si>
 </sst>
 </file>
@@ -2802,7 +2844,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A359" sqref="A359"/>
+      <selection pane="bottomLeft" activeCell="E365" sqref="E365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -9983,52 +10025,138 @@
       </c>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A359" s="5"/>
-      <c r="B359" s="13"/>
-      <c r="C359" s="4"/>
-      <c r="D359" s="2"/>
-      <c r="E359" s="2"/>
+      <c r="A359" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="B359" s="13">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="C359" s="4" t="s">
+        <v>774</v>
+      </c>
+      <c r="D359" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E359" s="2">
+        <v>60</v>
+      </c>
+      <c r="F359" s="1" t="s">
+        <v>775</v>
+      </c>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A360" s="5"/>
-      <c r="B360" s="13"/>
-      <c r="C360" s="4"/>
-      <c r="D360" s="2"/>
-      <c r="E360" s="2"/>
+      <c r="A360" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="B360" s="13">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="C360" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="D360" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E360" s="2">
+        <v>75</v>
+      </c>
+      <c r="F360" s="1" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="361" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A361" s="5"/>
-      <c r="B361" s="13"/>
-      <c r="C361" s="4"/>
-      <c r="D361" s="2"/>
-      <c r="E361" s="2"/>
+      <c r="A361" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="B361" s="13">
+        <v>0.96527777777777779</v>
+      </c>
+      <c r="C361" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="D361" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E361" s="2">
+        <v>200</v>
+      </c>
+      <c r="F361" s="1" t="s">
+        <v>779</v>
+      </c>
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A362" s="5"/>
-      <c r="B362" s="13"/>
-      <c r="C362" s="4"/>
-      <c r="D362" s="2"/>
-      <c r="E362" s="2"/>
+      <c r="A362" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="B362" s="13">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C362" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="D362" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E362" s="2">
+        <v>55</v>
+      </c>
+      <c r="F362" s="1" t="s">
+        <v>781</v>
+      </c>
     </row>
     <row r="363" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A363" s="5"/>
-      <c r="B363" s="13"/>
-      <c r="C363" s="4"/>
-      <c r="D363" s="2"/>
-      <c r="E363" s="2"/>
+      <c r="A363" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="B363" s="13">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C363" s="4" t="s">
+        <v>782</v>
+      </c>
+      <c r="D363" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E363" s="2">
+        <v>65</v>
+      </c>
+      <c r="F363" s="1" t="s">
+        <v>783</v>
+      </c>
     </row>
     <row r="364" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A364" s="5"/>
-      <c r="B364" s="13"/>
-      <c r="C364" s="4"/>
-      <c r="D364" s="2"/>
-      <c r="E364" s="2"/>
+      <c r="A364" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="B364" s="13">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C364" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="D364" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E364" s="2">
+        <v>65</v>
+      </c>
+      <c r="F364" s="1" t="s">
+        <v>786</v>
+      </c>
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A365" s="5"/>
-      <c r="B365" s="13"/>
-      <c r="C365" s="4"/>
-      <c r="D365" s="2"/>
+      <c r="A365" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="B365" s="13">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="C365" s="4" t="s">
+        <v>787</v>
+      </c>
+      <c r="D365" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="E365" s="2"/>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.25">
@@ -10053,7 +10181,7 @@
       </c>
       <c r="E368" s="3">
         <f>SUM(E2:E367)</f>
-        <v>32255</v>
+        <v>32775</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
@@ -10064,7 +10192,7 @@
       </c>
       <c r="E369" s="3">
         <f>E368 / 60</f>
-        <v>537.58333333333337</v>
+        <v>546.25</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Login, Register, Profile Pages
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3522" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09D7700A-4097-4CAA-9D60-4FE1E3E2050E}"/>
+  <xr:revisionPtr revIDLastSave="3585" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8607612-A31E-4262-888F-F0400F544AA9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="802">
   <si>
     <t>Date</t>
   </si>
@@ -2399,7 +2399,49 @@
     <t>Validate Edge Cases on Both Email and Password Inputs and Display User Message</t>
   </si>
   <si>
-    <t>Send POST:/api/login</t>
+    <t>Send GET:/</t>
+  </si>
+  <si>
+    <t>Connect to Localhost API Root</t>
+  </si>
+  <si>
+    <t>Create Register Page</t>
+  </si>
+  <si>
+    <t>POST api/subscribe</t>
+  </si>
+  <si>
+    <t>Create Subscribe Route, Get Email Info from ENV, Configure Email Account with App Passwords, Send Email</t>
+  </si>
+  <si>
+    <t>Confirm Email Link</t>
+  </si>
+  <si>
+    <t>Create a Confim Link in the Email with JWT Token</t>
+  </si>
+  <si>
+    <t>Fix API Bugs</t>
+  </si>
+  <si>
+    <t>Refactor Steps of Authentication Login Register Btn Redirects to Register Page and Then Send Confirm Email</t>
+  </si>
+  <si>
+    <t>Create Register Page, Input Validation, Styling, Login Styling, Background and Gradients</t>
+  </si>
+  <si>
+    <t>17.03.2023</t>
+  </si>
+  <si>
+    <t>Create Profile Page</t>
+  </si>
+  <si>
+    <t>Encryption Paragraph</t>
+  </si>
+  <si>
+    <t>Research Frontend and Backend Hashing and Encryption</t>
+  </si>
+  <si>
+    <t>Create 16 Avatars, Profile Form, Backbround, Display Avatars Dynamically</t>
   </si>
 </sst>
 </file>
@@ -2840,11 +2882,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M624"/>
+  <dimension ref="A1:M631"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E365" sqref="E365"/>
+      <pane ySplit="1" topLeftCell="A340" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F372" sqref="F372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -10157,101 +10199,205 @@
       <c r="D365" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E365" s="2"/>
+      <c r="E365" s="2">
+        <v>85</v>
+      </c>
+      <c r="F365" s="1" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A366" s="5"/>
-      <c r="B366" s="13"/>
-      <c r="C366" s="4"/>
-      <c r="D366" s="2"/>
-      <c r="E366" s="2"/>
+      <c r="A366" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="B366" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="C366" s="4" t="s">
+        <v>790</v>
+      </c>
+      <c r="D366" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E366" s="2">
+        <v>140</v>
+      </c>
+      <c r="F366" s="1" t="s">
+        <v>791</v>
+      </c>
     </row>
     <row r="367" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A367" s="5"/>
-      <c r="B367" s="13"/>
-      <c r="C367" s="4"/>
-      <c r="D367" s="2"/>
-      <c r="E367" s="2"/>
+      <c r="A367" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="B367" s="13">
+        <v>0.875</v>
+      </c>
+      <c r="C367" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="D367" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E367" s="2">
+        <v>50</v>
+      </c>
+      <c r="F367" s="1" t="s">
+        <v>793</v>
+      </c>
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A368" s="10"/>
-      <c r="B368" s="10"/>
-      <c r="D368" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E368" s="3">
-        <f>SUM(E2:E367)</f>
-        <v>32775</v>
-      </c>
-    </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A369" s="10"/>
-      <c r="B369" s="10"/>
-      <c r="D369" s="3" t="s">
+      <c r="A368" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="B368" s="13">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="C368" s="4" t="s">
+        <v>794</v>
+      </c>
+      <c r="D368" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E368" s="2">
+        <v>30</v>
+      </c>
+      <c r="F368" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="B369" s="13">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="C369" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="D369" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E369" s="2">
         <v>210</v>
       </c>
-      <c r="E369" s="3">
-        <f>E368 / 60</f>
-        <v>546.25</v>
-      </c>
-    </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A370" s="10"/>
-      <c r="B370" s="10"/>
-    </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A371" s="10"/>
-      <c r="B371" s="10"/>
-    </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A372" s="10"/>
-      <c r="B372" s="10"/>
-    </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A373" s="10"/>
-      <c r="B373" s="10"/>
-    </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A374" s="10"/>
-      <c r="B374" s="10"/>
-    </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F369" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B370" s="13">
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="C370" s="4" t="s">
+        <v>799</v>
+      </c>
+      <c r="D370" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E370" s="2">
+        <v>90</v>
+      </c>
+      <c r="F370" s="1" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A371" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B371" s="13">
+        <v>0.1423611111111111</v>
+      </c>
+      <c r="C371" s="4" t="s">
+        <v>798</v>
+      </c>
+      <c r="D371" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E371" s="2">
+        <v>135</v>
+      </c>
+      <c r="F371" s="1" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A372" s="5"/>
+      <c r="B372" s="13"/>
+      <c r="C372" s="4"/>
+      <c r="D372" s="2"/>
+      <c r="E372" s="2"/>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A373" s="5"/>
+      <c r="B373" s="13"/>
+      <c r="C373" s="4"/>
+      <c r="D373" s="2"/>
+      <c r="E373" s="2"/>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A374" s="5"/>
+      <c r="B374" s="13"/>
+      <c r="C374" s="4"/>
+      <c r="D374" s="2"/>
+      <c r="E374" s="2"/>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A375" s="10"/>
       <c r="B375" s="10"/>
-    </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D375" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E375" s="3">
+        <f>SUM(E2:E374)</f>
+        <v>33515</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A376" s="10"/>
       <c r="B376" s="10"/>
-    </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D376" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E376" s="3">
+        <f>E375 / 60</f>
+        <v>558.58333333333337</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A377" s="10"/>
       <c r="B377" s="10"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A378" s="10"/>
       <c r="B378" s="10"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A379" s="10"/>
       <c r="B379" s="10"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A380" s="10"/>
       <c r="B380" s="10"/>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A381" s="10"/>
       <c r="B381" s="10"/>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A382" s="10"/>
       <c r="B382" s="10"/>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383" s="10"/>
       <c r="B383" s="10"/>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384" s="10"/>
       <c r="B384" s="10"/>
     </row>
@@ -11214,6 +11360,34 @@
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" s="10"/>
       <c r="B624" s="10"/>
+    </row>
+    <row r="625" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A625" s="10"/>
+      <c r="B625" s="10"/>
+    </row>
+    <row r="626" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A626" s="10"/>
+      <c r="B626" s="10"/>
+    </row>
+    <row r="627" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A627" s="10"/>
+      <c r="B627" s="10"/>
+    </row>
+    <row r="628" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A628" s="10"/>
+      <c r="B628" s="10"/>
+    </row>
+    <row r="629" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A629" s="10"/>
+      <c r="B629" s="10"/>
+    </row>
+    <row r="630" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A630" s="10"/>
+      <c r="B630" s="10"/>
+    </row>
+    <row r="631" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A631" s="10"/>
+      <c r="B631" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Login - Logout Process
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3593" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DF08A3D-7D51-4864-9C39-DB947FCD6DD2}"/>
+  <xr:revisionPtr revIDLastSave="3616" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89206204-E263-434C-98B0-DF9AE25339B3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="808">
   <si>
     <t>Date</t>
   </si>
@@ -2445,6 +2445,21 @@
   </si>
   <si>
     <t>Complete Form Validation, Avatar Selection, Valid Dates and Formats, Autocomplete Countries</t>
+  </si>
+  <si>
+    <t>Register a User</t>
+  </si>
+  <si>
+    <t>Send Subsrcibe Request and Send User Info Via JWT, Create User and Profile</t>
+  </si>
+  <si>
+    <t>18.03.2023</t>
+  </si>
+  <si>
+    <t>Complete Login / Logout Process</t>
+  </si>
+  <si>
+    <t>Validate Registration on Backend, Send Token, Hash Password, Login User, Logout User</t>
   </si>
 </sst>
 </file>
@@ -2885,11 +2900,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M631"/>
+  <dimension ref="A1:M638"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A340" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A373" sqref="A373"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C375" sqref="C375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -10350,68 +10365,115 @@
       </c>
     </row>
     <row r="373" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A373" s="5"/>
-      <c r="B373" s="13"/>
-      <c r="C373" s="4"/>
-      <c r="D373" s="2"/>
-      <c r="E373" s="2"/>
+      <c r="A373" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B373" s="13">
+        <v>0.9375</v>
+      </c>
+      <c r="C373" s="4" t="s">
+        <v>803</v>
+      </c>
+      <c r="D373" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E373" s="2">
+        <v>105</v>
+      </c>
+      <c r="F373" s="1" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row r="374" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A374" s="5"/>
-      <c r="B374" s="13"/>
-      <c r="C374" s="4"/>
-      <c r="D374" s="2"/>
-      <c r="E374" s="2"/>
+      <c r="A374" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="B374" s="13">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="C374" s="4" t="s">
+        <v>806</v>
+      </c>
+      <c r="D374" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E374" s="2">
+        <v>220</v>
+      </c>
+      <c r="F374" s="1" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="375" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A375" s="10"/>
-      <c r="B375" s="10"/>
-      <c r="D375" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E375" s="3">
-        <f>SUM(E2:E374)</f>
-        <v>33745</v>
-      </c>
+      <c r="A375" s="5"/>
+      <c r="B375" s="13"/>
+      <c r="C375" s="4"/>
+      <c r="D375" s="2"/>
+      <c r="E375" s="2"/>
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A376" s="10"/>
-      <c r="B376" s="10"/>
-      <c r="D376" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E376" s="3">
-        <f>E375 / 60</f>
-        <v>562.41666666666663</v>
-      </c>
+      <c r="A376" s="5"/>
+      <c r="B376" s="13"/>
+      <c r="C376" s="4"/>
+      <c r="D376" s="2"/>
+      <c r="E376" s="2"/>
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A377" s="10"/>
-      <c r="B377" s="10"/>
+      <c r="A377" s="5"/>
+      <c r="B377" s="13"/>
+      <c r="C377" s="4"/>
+      <c r="D377" s="2"/>
+      <c r="E377" s="2"/>
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A378" s="10"/>
-      <c r="B378" s="10"/>
+      <c r="A378" s="5"/>
+      <c r="B378" s="13"/>
+      <c r="C378" s="4"/>
+      <c r="D378" s="2"/>
+      <c r="E378" s="2"/>
     </row>
     <row r="379" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A379" s="10"/>
-      <c r="B379" s="10"/>
+      <c r="A379" s="5"/>
+      <c r="B379" s="13"/>
+      <c r="C379" s="4"/>
+      <c r="D379" s="2"/>
+      <c r="E379" s="2"/>
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A380" s="10"/>
-      <c r="B380" s="10"/>
+      <c r="A380" s="5"/>
+      <c r="B380" s="13"/>
+      <c r="C380" s="4"/>
+      <c r="D380" s="2"/>
+      <c r="E380" s="2"/>
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A381" s="10"/>
-      <c r="B381" s="10"/>
+      <c r="A381" s="5"/>
+      <c r="B381" s="13"/>
+      <c r="C381" s="4"/>
+      <c r="D381" s="2"/>
+      <c r="E381" s="2"/>
     </row>
     <row r="382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A382" s="10"/>
       <c r="B382" s="10"/>
+      <c r="D382" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E382" s="3">
+        <f>SUM(E2:E381)</f>
+        <v>34070</v>
+      </c>
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383" s="10"/>
       <c r="B383" s="10"/>
+      <c r="D383" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E383" s="3">
+        <f>E382 / 60</f>
+        <v>567.83333333333337</v>
+      </c>
     </row>
     <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384" s="10"/>
@@ -11404,6 +11466,34 @@
     <row r="631" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A631" s="10"/>
       <c r="B631" s="10"/>
+    </row>
+    <row r="632" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A632" s="10"/>
+      <c r="B632" s="10"/>
+    </row>
+    <row r="633" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A633" s="10"/>
+      <c r="B633" s="10"/>
+    </row>
+    <row r="634" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A634" s="10"/>
+      <c r="B634" s="10"/>
+    </row>
+    <row r="635" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A635" s="10"/>
+      <c r="B635" s="10"/>
+    </row>
+    <row r="636" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A636" s="10"/>
+      <c r="B636" s="10"/>
+    </row>
+    <row r="637" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A637" s="10"/>
+      <c r="B637" s="10"/>
+    </row>
+    <row r="638" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A638" s="10"/>
+      <c r="B638" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Compose - Highlight Current Bar and Paginate Overflow
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3616" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89206204-E263-434C-98B0-DF9AE25339B3}"/>
+  <xr:revisionPtr revIDLastSave="3654" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89F7C281-4EEF-42A9-A468-834E790F473E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="820">
   <si>
     <t>Date</t>
   </si>
@@ -2460,6 +2460,42 @@
   </si>
   <si>
     <t>Validate Registration on Backend, Send Token, Hash Password, Login User, Logout User</t>
+  </si>
+  <si>
+    <t>Document Backend</t>
+  </si>
+  <si>
+    <t>API Routes Diagram, Explanation, 2 Phase Registration, Code Snippets</t>
+  </si>
+  <si>
+    <t>22.03.2023</t>
+  </si>
+  <si>
+    <t>Compose - Restructure Tab Format</t>
+  </si>
+  <si>
+    <t>Complete Restructure, Commenting, Debbuging…</t>
+  </si>
+  <si>
+    <t>Compose - Game Loop Timing</t>
+  </si>
+  <si>
+    <t>Calculate Loop Timing from Music Tab Tempo</t>
+  </si>
+  <si>
+    <t>Compose - Validate Tab</t>
+  </si>
+  <si>
+    <t>Compose - Focus Bar 1</t>
+  </si>
+  <si>
+    <t>Center Single Line Current Bar</t>
+  </si>
+  <si>
+    <t>Compose - Focus Bar 2</t>
+  </si>
+  <si>
+    <t>Center Multi Line Current Bar</t>
   </si>
 </sst>
 </file>
@@ -2900,11 +2936,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M638"/>
+  <dimension ref="A1:M639"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C375" sqref="C375"/>
+      <selection pane="bottomLeft" activeCell="E380" sqref="E380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -10405,45 +10441,114 @@
       </c>
     </row>
     <row r="375" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A375" s="5"/>
-      <c r="B375" s="13"/>
-      <c r="C375" s="4"/>
-      <c r="D375" s="2"/>
-      <c r="E375" s="2"/>
+      <c r="A375" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="B375" s="13">
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="C375" s="4" t="s">
+        <v>808</v>
+      </c>
+      <c r="D375" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E375" s="2">
+        <v>90</v>
+      </c>
+      <c r="F375" s="1" t="s">
+        <v>809</v>
+      </c>
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A376" s="5"/>
-      <c r="B376" s="13"/>
-      <c r="C376" s="4"/>
-      <c r="D376" s="2"/>
-      <c r="E376" s="2"/>
+      <c r="A376" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="B376" s="13">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="C376" s="4" t="s">
+        <v>811</v>
+      </c>
+      <c r="D376" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E376" s="2">
+        <v>220</v>
+      </c>
+      <c r="F376" s="1" t="s">
+        <v>812</v>
+      </c>
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A377" s="5"/>
-      <c r="B377" s="13"/>
-      <c r="C377" s="4"/>
-      <c r="D377" s="2"/>
-      <c r="E377" s="2"/>
+      <c r="A377" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="B377" s="13">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C377" s="4" t="s">
+        <v>813</v>
+      </c>
+      <c r="D377" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E377" s="2">
+        <v>25</v>
+      </c>
+      <c r="F377" s="1" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A378" s="5"/>
-      <c r="B378" s="13"/>
-      <c r="C378" s="4"/>
-      <c r="D378" s="2"/>
-      <c r="E378" s="2"/>
+      <c r="A378" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="B378" s="13">
+        <v>0.6875</v>
+      </c>
+      <c r="C378" s="4" t="s">
+        <v>816</v>
+      </c>
+      <c r="D378" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E378" s="2">
+        <v>75</v>
+      </c>
+      <c r="F378" s="1" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="379" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A379" s="5"/>
-      <c r="B379" s="13"/>
-      <c r="C379" s="4"/>
-      <c r="D379" s="2"/>
-      <c r="E379" s="2"/>
+      <c r="A379" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="B379" s="13">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="C379" s="4" t="s">
+        <v>818</v>
+      </c>
+      <c r="D379" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E379" s="2">
+        <v>245</v>
+      </c>
+      <c r="F379" s="1" t="s">
+        <v>819</v>
+      </c>
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A380" s="5"/>
       <c r="B380" s="13"/>
-      <c r="C380" s="4"/>
-      <c r="D380" s="2"/>
+      <c r="C380" s="4" t="s">
+        <v>815</v>
+      </c>
+      <c r="D380" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="E380" s="2"/>
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.25">
@@ -10454,30 +10559,33 @@
       <c r="E381" s="2"/>
     </row>
     <row r="382" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A382" s="10"/>
-      <c r="B382" s="10"/>
-      <c r="D382" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E382" s="3">
-        <f>SUM(E2:E381)</f>
-        <v>34070</v>
-      </c>
+      <c r="A382" s="5"/>
+      <c r="B382" s="13"/>
+      <c r="C382" s="4"/>
+      <c r="D382" s="2"/>
+      <c r="E382" s="2"/>
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383" s="10"/>
       <c r="B383" s="10"/>
       <c r="D383" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E383" s="3">
-        <f>E382 / 60</f>
-        <v>567.83333333333337</v>
+        <f>SUM(E2:E382)</f>
+        <v>34725</v>
       </c>
     </row>
     <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384" s="10"/>
       <c r="B384" s="10"/>
+      <c r="D384" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E384" s="3">
+        <f>E383 / 60</f>
+        <v>578.75</v>
+      </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" s="10"/>
@@ -11494,6 +11602,10 @@
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A638" s="10"/>
       <c r="B638" s="10"/>
+    </row>
+    <row r="639" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A639" s="10"/>
+      <c r="B639" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Play and Stop Notes
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3654" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89F7C281-4EEF-42A9-A468-834E790F473E}"/>
+  <xr:revisionPtr revIDLastSave="3773" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D47D4162-5554-44B6-A118-055A68C46A91}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="847">
   <si>
     <t>Date</t>
   </si>
@@ -2495,7 +2495,88 @@
     <t>Compose - Focus Bar 2</t>
   </si>
   <si>
-    <t>Center Multi Line Current Bar</t>
+    <t>23.03.2023</t>
+  </si>
+  <si>
+    <t>Compose - Highlight Note</t>
+  </si>
+  <si>
+    <t>Center Multi Line Current Bar and Highlight Current Bar</t>
+  </si>
+  <si>
+    <t>Highlight Current Notes</t>
+  </si>
+  <si>
+    <t>Validate Tab Formatting before Load and Create Error Message</t>
+  </si>
+  <si>
+    <t>Compose - Name of Tempos</t>
+  </si>
+  <si>
+    <t>Find Appropriate Latin Tempo Names for BPM Ranges</t>
+  </si>
+  <si>
+    <t>Compose - Play Notes</t>
+  </si>
+  <si>
+    <t>Compose - Stop Notes</t>
+  </si>
+  <si>
+    <t>Safe Redirect</t>
+  </si>
+  <si>
+    <t>Redirect Utility Function: Takes URL as Parameter, Saves User and Token on Local Storage, Redirect Page, Copies User in Global Var, Delete Storage</t>
+  </si>
+  <si>
+    <t>Registration - Email Duplicates</t>
+  </si>
+  <si>
+    <t>Check DB for Duplicated User Emails Before Redirecting to Profile Page</t>
+  </si>
+  <si>
+    <t>Compose - Change Tempo</t>
+  </si>
+  <si>
+    <t>Compose - Change Title/Artist</t>
+  </si>
+  <si>
+    <t>Compose - Editable Notes</t>
+  </si>
+  <si>
+    <t>Compose - DB Properties</t>
+  </si>
+  <si>
+    <t>isPublised, No Album Cover Image / Avatar or Album Image Cover URL</t>
+  </si>
+  <si>
+    <t>Compose - Repeat Section</t>
+  </si>
+  <si>
+    <t>Compose - Bar Pagination</t>
+  </si>
+  <si>
+    <t>Compose - Duration Notation</t>
+  </si>
+  <si>
+    <t>Compose - Save Tab</t>
+  </si>
+  <si>
+    <t>Compose - Load Tab</t>
+  </si>
+  <si>
+    <t>Compose - Record Guitar Input</t>
+  </si>
+  <si>
+    <t>Compose - Note Placement Warning</t>
+  </si>
+  <si>
+    <t>Index - Load User Info from DB</t>
+  </si>
+  <si>
+    <t>Find Given Point in Current Bar's Start Position and Play Note Audio</t>
+  </si>
+  <si>
+    <t>Calculate Note Stop Delay and Call Timer for Each Playing Note</t>
   </si>
 </sst>
 </file>
@@ -2936,11 +3017,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M639"/>
+  <dimension ref="A1:M656"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E380" sqref="E380"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F385" sqref="F385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -10537,181 +10618,388 @@
         <v>245</v>
       </c>
       <c r="F379" s="1" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A380" s="5" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A380" s="5"/>
-      <c r="B380" s="13"/>
+      <c r="B380" s="13">
+        <v>1.7361111111111112E-2</v>
+      </c>
       <c r="C380" s="4" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="D380" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E380" s="2"/>
+      <c r="E380" s="2">
+        <v>85</v>
+      </c>
+      <c r="F380" s="1" t="s">
+        <v>822</v>
+      </c>
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A381" s="5"/>
-      <c r="B381" s="13"/>
-      <c r="C381" s="4"/>
-      <c r="D381" s="2"/>
-      <c r="E381" s="2"/>
+      <c r="A381" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B381" s="13">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="C381" s="4" t="s">
+        <v>815</v>
+      </c>
+      <c r="D381" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E381" s="2">
+        <v>180</v>
+      </c>
+      <c r="F381" s="1" t="s">
+        <v>823</v>
+      </c>
     </row>
     <row r="382" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A382" s="5"/>
-      <c r="B382" s="13"/>
-      <c r="C382" s="4"/>
-      <c r="D382" s="2"/>
-      <c r="E382" s="2"/>
+      <c r="A382" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B382" s="13">
+        <v>0.20138888888888887</v>
+      </c>
+      <c r="C382" s="4" t="s">
+        <v>824</v>
+      </c>
+      <c r="D382" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E382" s="2">
+        <v>20</v>
+      </c>
+      <c r="F382" s="1" t="s">
+        <v>825</v>
+      </c>
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A383" s="10"/>
-      <c r="B383" s="10"/>
-      <c r="D383" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E383" s="3">
-        <f>SUM(E2:E382)</f>
-        <v>34725</v>
+      <c r="A383" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B383" s="13">
+        <v>0.21875</v>
+      </c>
+      <c r="C383" s="4" t="s">
+        <v>826</v>
+      </c>
+      <c r="D383" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E383" s="2">
+        <v>40</v>
+      </c>
+      <c r="F383" s="1" t="s">
+        <v>845</v>
       </c>
     </row>
     <row r="384" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A384" s="10"/>
-      <c r="B384" s="10"/>
-      <c r="D384" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E384" s="3">
-        <f>E383 / 60</f>
-        <v>578.75</v>
-      </c>
-    </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A385" s="10"/>
-      <c r="B385" s="10"/>
-    </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A386" s="10"/>
-      <c r="B386" s="10"/>
-    </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A387" s="10"/>
-      <c r="B387" s="10"/>
-    </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A388" s="10"/>
-      <c r="B388" s="10"/>
-    </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A389" s="10"/>
-      <c r="B389" s="10"/>
-    </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A390" s="10"/>
-      <c r="B390" s="10"/>
-    </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A391" s="10"/>
-      <c r="B391" s="10"/>
-    </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A392" s="10"/>
-      <c r="B392" s="10"/>
-    </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A393" s="10"/>
-      <c r="B393" s="10"/>
-    </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A394" s="10"/>
-      <c r="B394" s="10"/>
-    </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A395" s="10"/>
-      <c r="B395" s="10"/>
-    </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A396" s="10"/>
-      <c r="B396" s="10"/>
-    </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A397" s="10"/>
-      <c r="B397" s="10"/>
-    </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A398" s="10"/>
-      <c r="B398" s="10"/>
-    </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A399" s="10"/>
-      <c r="B399" s="10"/>
-    </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B384" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C384" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D384" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E384" s="2">
+        <v>90</v>
+      </c>
+      <c r="F384" s="1" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A385" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B385" s="13">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="C385" s="4" t="s">
+        <v>843</v>
+      </c>
+      <c r="D385" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E385" s="2"/>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A386" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B386" s="13"/>
+      <c r="C386" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="D386" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E386" s="2"/>
+      <c r="F386" s="1" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A387" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B387" s="13"/>
+      <c r="C387" s="4" t="s">
+        <v>830</v>
+      </c>
+      <c r="D387" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E387" s="2"/>
+      <c r="F387" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A388" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B388" s="13"/>
+      <c r="C388" s="4" t="s">
+        <v>839</v>
+      </c>
+      <c r="D388" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E388" s="2"/>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A389" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B389" s="13"/>
+      <c r="C389" s="4" t="s">
+        <v>832</v>
+      </c>
+      <c r="D389" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E389" s="2"/>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A390" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B390" s="13"/>
+      <c r="C390" s="4" t="s">
+        <v>833</v>
+      </c>
+      <c r="D390" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E390" s="2"/>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A391" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B391" s="13"/>
+      <c r="C391" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="D391" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E391" s="2"/>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A392" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B392" s="13"/>
+      <c r="C392" s="4" t="s">
+        <v>835</v>
+      </c>
+      <c r="D392" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E392" s="2"/>
+      <c r="F392" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A393" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B393" s="13"/>
+      <c r="C393" s="4" t="s">
+        <v>838</v>
+      </c>
+      <c r="D393" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E393" s="2"/>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A394" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B394" s="13"/>
+      <c r="C394" s="4" t="s">
+        <v>837</v>
+      </c>
+      <c r="D394" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E394" s="2"/>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A395" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B395" s="13"/>
+      <c r="C395" s="4" t="s">
+        <v>840</v>
+      </c>
+      <c r="D395" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E395" s="2"/>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A396" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B396" s="13"/>
+      <c r="C396" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="D396" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E396" s="2"/>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A397" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B397" s="13"/>
+      <c r="C397" s="4" t="s">
+        <v>842</v>
+      </c>
+      <c r="D397" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E397" s="2"/>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A398" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="B398" s="13"/>
+      <c r="C398" s="4" t="s">
+        <v>844</v>
+      </c>
+      <c r="D398" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E398" s="2"/>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A399" s="5"/>
+      <c r="B399" s="13"/>
+      <c r="C399" s="4"/>
+      <c r="D399" s="2"/>
+      <c r="E399" s="2"/>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A400" s="10"/>
       <c r="B400" s="10"/>
-    </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D400" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E400" s="3">
+        <f>SUM(E2:E399)</f>
+        <v>35140</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A401" s="10"/>
       <c r="B401" s="10"/>
-    </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D401" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E401" s="3">
+        <f>E400 / 60</f>
+        <v>585.66666666666663</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402" s="10"/>
       <c r="B402" s="10"/>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403" s="10"/>
       <c r="B403" s="10"/>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404" s="10"/>
       <c r="B404" s="10"/>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405" s="10"/>
       <c r="B405" s="10"/>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406" s="10"/>
       <c r="B406" s="10"/>
     </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407" s="10"/>
       <c r="B407" s="10"/>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408" s="10"/>
       <c r="B408" s="10"/>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A409" s="10"/>
       <c r="B409" s="10"/>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A410" s="10"/>
       <c r="B410" s="10"/>
     </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A411" s="10"/>
       <c r="B411" s="10"/>
     </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A412" s="10"/>
       <c r="B412" s="10"/>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A413" s="10"/>
       <c r="B413" s="10"/>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A414" s="10"/>
       <c r="B414" s="10"/>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415" s="10"/>
       <c r="B415" s="10"/>
     </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A416" s="10"/>
       <c r="B416" s="10"/>
     </row>
@@ -11606,6 +11894,74 @@
     <row r="639" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A639" s="10"/>
       <c r="B639" s="10"/>
+    </row>
+    <row r="640" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A640" s="10"/>
+      <c r="B640" s="10"/>
+    </row>
+    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A641" s="10"/>
+      <c r="B641" s="10"/>
+    </row>
+    <row r="642" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A642" s="10"/>
+      <c r="B642" s="10"/>
+    </row>
+    <row r="643" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A643" s="10"/>
+      <c r="B643" s="10"/>
+    </row>
+    <row r="644" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A644" s="10"/>
+      <c r="B644" s="10"/>
+    </row>
+    <row r="645" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A645" s="10"/>
+      <c r="B645" s="10"/>
+    </row>
+    <row r="646" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A646" s="10"/>
+      <c r="B646" s="10"/>
+    </row>
+    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A647" s="10"/>
+      <c r="B647" s="10"/>
+    </row>
+    <row r="648" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A648" s="10"/>
+      <c r="B648" s="10"/>
+    </row>
+    <row r="649" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A649" s="10"/>
+      <c r="B649" s="10"/>
+    </row>
+    <row r="650" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A650" s="10"/>
+      <c r="B650" s="10"/>
+    </row>
+    <row r="651" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A651" s="10"/>
+      <c r="B651" s="10"/>
+    </row>
+    <row r="652" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A652" s="10"/>
+      <c r="B652" s="10"/>
+    </row>
+    <row r="653" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A653" s="10"/>
+      <c r="B653" s="10"/>
+    </row>
+    <row r="654" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A654" s="10"/>
+      <c r="B654" s="10"/>
+    </row>
+    <row r="655" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A655" s="10"/>
+      <c r="B655" s="10"/>
+    </row>
+    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A656" s="10"/>
+      <c r="B656" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Style Compose, Add Buttons, Add Music Notation, Editable Tab Properties
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3773" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D47D4162-5554-44B6-A118-055A68C46A91}"/>
+  <xr:revisionPtr revIDLastSave="3814" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A33B373A-F320-4440-A5AD-A7F0C6A6FB72}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="856">
   <si>
     <t>Date</t>
   </si>
@@ -2577,6 +2577,33 @@
   </si>
   <si>
     <t>Calculate Note Stop Delay and Call Timer for Each Playing Note</t>
+  </si>
+  <si>
+    <t>Colour Notes that Are Impossible to Play with Red (Eg.: Same Starting Time E0, E2)</t>
+  </si>
+  <si>
+    <t>Compose - Tab CSS</t>
+  </si>
+  <si>
+    <t>Neumorphic Style for Tabs</t>
+  </si>
+  <si>
+    <t>Create Music Notation Icons and Place them in the Tablature</t>
+  </si>
+  <si>
+    <t>Make Tempo Changeable, Reset Game Loop Timer, Add Rest of the Buttons</t>
+  </si>
+  <si>
+    <t>User Can Change Title and Author Attributes of a Tablature</t>
+  </si>
+  <si>
+    <t>24.03.2023</t>
+  </si>
+  <si>
+    <t>Create Sample Tab</t>
+  </si>
+  <si>
+    <t>Hard Code a Test Tab: Metallica | Master of Puppets Intro</t>
   </si>
 </sst>
 </file>
@@ -2714,10 +2741,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3017,11 +3040,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M656"/>
+  <dimension ref="A1:M658"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F385" sqref="F385"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A369" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A393" sqref="A393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -10734,115 +10757,162 @@
       <c r="D385" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E385" s="2"/>
+      <c r="E385" s="2">
+        <v>10</v>
+      </c>
+      <c r="F385" s="1" t="s">
+        <v>847</v>
+      </c>
     </row>
     <row r="386" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A386" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="B386" s="13"/>
+      <c r="B386" s="13">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="C386" s="4" t="s">
-        <v>828</v>
+        <v>848</v>
       </c>
       <c r="D386" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E386" s="2"/>
+      <c r="E386" s="2">
+        <v>45</v>
+      </c>
       <c r="F386" s="1" t="s">
-        <v>829</v>
+        <v>849</v>
       </c>
     </row>
     <row r="387" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A387" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="B387" s="13"/>
+      <c r="B387" s="13">
+        <v>0.68055555555555547</v>
+      </c>
       <c r="C387" s="4" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D387" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E387" s="2"/>
+      <c r="E387" s="2">
+        <v>40</v>
+      </c>
       <c r="F387" s="1" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="388" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A388" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="B388" s="13"/>
+      <c r="B388" s="13">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="C388" s="4" t="s">
-        <v>839</v>
+        <v>830</v>
       </c>
       <c r="D388" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E388" s="2"/>
+      <c r="E388" s="2">
+        <v>35</v>
+      </c>
+      <c r="F388" s="1" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="B389" s="13"/>
+      <c r="B389" s="13">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="C389" s="4" t="s">
-        <v>832</v>
+        <v>839</v>
       </c>
       <c r="D389" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E389" s="2"/>
+      <c r="E389" s="2">
+        <v>150</v>
+      </c>
+      <c r="F389" s="1" t="s">
+        <v>850</v>
+      </c>
     </row>
     <row r="390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A390" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="B390" s="13"/>
+      <c r="B390" s="13">
+        <v>0.87152777777777779</v>
+      </c>
       <c r="C390" s="4" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D390" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E390" s="2"/>
+      <c r="E390" s="2">
+        <v>90</v>
+      </c>
+      <c r="F390" s="1" t="s">
+        <v>851</v>
+      </c>
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A391" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="B391" s="13"/>
+      <c r="B391" s="13">
+        <v>0.95138888888888884</v>
+      </c>
       <c r="C391" s="4" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D391" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E391" s="2"/>
+      <c r="E391" s="2">
+        <v>10</v>
+      </c>
+      <c r="F391" s="1" t="s">
+        <v>852</v>
+      </c>
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A392" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="B392" s="13"/>
+      <c r="B392" s="13">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="C392" s="4" t="s">
-        <v>835</v>
+        <v>854</v>
       </c>
       <c r="D392" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E392" s="2"/>
+      <c r="E392" s="2">
+        <v>50</v>
+      </c>
       <c r="F392" s="1" t="s">
-        <v>836</v>
+        <v>855</v>
       </c>
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393" s="5" t="s">
-        <v>819</v>
-      </c>
-      <c r="B393" s="13"/>
+        <v>853</v>
+      </c>
+      <c r="B393" s="13">
+        <v>0</v>
+      </c>
       <c r="C393" s="4" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="D393" s="2" t="s">
         <v>162</v>
@@ -10850,25 +10920,24 @@
       <c r="E393" s="2"/>
     </row>
     <row r="394" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A394" s="5" t="s">
-        <v>819</v>
-      </c>
+      <c r="A394" s="5"/>
       <c r="B394" s="13"/>
       <c r="C394" s="4" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D394" s="2" t="s">
         <v>162</v>
       </c>
       <c r="E394" s="2"/>
+      <c r="F394" s="1" t="s">
+        <v>836</v>
+      </c>
     </row>
     <row r="395" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A395" s="5" t="s">
-        <v>819</v>
-      </c>
+      <c r="A395" s="5"/>
       <c r="B395" s="13"/>
       <c r="C395" s="4" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D395" s="2" t="s">
         <v>162</v>
@@ -10876,12 +10945,10 @@
       <c r="E395" s="2"/>
     </row>
     <row r="396" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A396" s="5" t="s">
-        <v>819</v>
-      </c>
+      <c r="A396" s="5"/>
       <c r="B396" s="13"/>
       <c r="C396" s="4" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D396" s="2" t="s">
         <v>162</v>
@@ -10889,12 +10956,10 @@
       <c r="E396" s="2"/>
     </row>
     <row r="397" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A397" s="5" t="s">
-        <v>819</v>
-      </c>
+      <c r="A397" s="5"/>
       <c r="B397" s="13"/>
       <c r="C397" s="4" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="D397" s="2" t="s">
         <v>162</v>
@@ -10902,12 +10967,10 @@
       <c r="E397" s="2"/>
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A398" s="5" t="s">
-        <v>819</v>
-      </c>
+      <c r="A398" s="5"/>
       <c r="B398" s="13"/>
       <c r="C398" s="4" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="D398" s="2" t="s">
         <v>162</v>
@@ -10917,39 +10980,53 @@
     <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399" s="5"/>
       <c r="B399" s="13"/>
-      <c r="C399" s="4"/>
-      <c r="D399" s="2"/>
+      <c r="C399" s="4" t="s">
+        <v>842</v>
+      </c>
+      <c r="D399" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="E399" s="2"/>
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A400" s="10"/>
-      <c r="B400" s="10"/>
-      <c r="D400" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E400" s="3">
-        <f>SUM(E2:E399)</f>
-        <v>35140</v>
-      </c>
+      <c r="A400" s="5"/>
+      <c r="B400" s="13"/>
+      <c r="C400" s="4" t="s">
+        <v>844</v>
+      </c>
+      <c r="D400" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E400" s="2"/>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A401" s="10"/>
-      <c r="B401" s="10"/>
-      <c r="D401" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E401" s="3">
-        <f>E400 / 60</f>
-        <v>585.66666666666663</v>
-      </c>
+      <c r="A401" s="5"/>
+      <c r="B401" s="13"/>
+      <c r="C401" s="4"/>
+      <c r="D401" s="2"/>
+      <c r="E401" s="2"/>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402" s="10"/>
       <c r="B402" s="10"/>
+      <c r="D402" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E402" s="3">
+        <f>SUM(E2:E401)</f>
+        <v>35570</v>
+      </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403" s="10"/>
       <c r="B403" s="10"/>
+      <c r="D403" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E403" s="3">
+        <f>E402 / 60</f>
+        <v>592.83333333333337</v>
+      </c>
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404" s="10"/>
@@ -11962,6 +12039,14 @@
     <row r="656" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A656" s="10"/>
       <c r="B656" s="10"/>
+    </row>
+    <row r="657" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A657" s="10"/>
+      <c r="B657" s="10"/>
+    </row>
+    <row r="658" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A658" s="10"/>
+      <c r="B658" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Edit Tabs and Repeat Play from Sections
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3814" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A33B373A-F320-4440-A5AD-A7F0C6A6FB72}"/>
+  <xr:revisionPtr revIDLastSave="3870" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35313108-6602-4AC5-8A07-BA7BAEFC1411}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="867">
   <si>
     <t>Date</t>
   </si>
@@ -2540,9 +2540,6 @@
     <t>Compose - Change Title/Artist</t>
   </si>
   <si>
-    <t>Compose - Editable Notes</t>
-  </si>
-  <si>
     <t>Compose - DB Properties</t>
   </si>
   <si>
@@ -2604,6 +2601,42 @@
   </si>
   <si>
     <t>Hard Code a Test Tab: Metallica | Master of Puppets Intro</t>
+  </si>
+  <si>
+    <t>Step Forward, Backward, Display Indexing, Disable Buttons</t>
+  </si>
+  <si>
+    <t>Compose - Editable Notes 1</t>
+  </si>
+  <si>
+    <t>Toggle Edit Btn, Scale Note Under Cursor, Toggle Editability</t>
+  </si>
+  <si>
+    <t>Compose - Editable Notes 2</t>
+  </si>
+  <si>
+    <t>Dynamically Create an Edit Note Form that Reads Values from the Note Clicked</t>
+  </si>
+  <si>
+    <t>Compose - Editable Notes 3</t>
+  </si>
+  <si>
+    <t>Add, Modify and Delete Notes from the Tablature Sheet</t>
+  </si>
+  <si>
+    <t>Compose - Editable Notes 4</t>
+  </si>
+  <si>
+    <t>Move Notes and Delete / Insert Bars, Create Action History and Undo Feature</t>
+  </si>
+  <si>
+    <t>25.03.2023</t>
+  </si>
+  <si>
+    <t>Repeat Toggle Button, Inputs and Validations, Manipulate Play Run</t>
+  </si>
+  <si>
+    <t>Compose - Metronome Volume</t>
   </si>
 </sst>
 </file>
@@ -2741,6 +2774,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3040,11 +3077,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M658"/>
+  <dimension ref="A1:M662"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A369" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A393" sqref="A393"/>
+      <pane ySplit="1" topLeftCell="A377" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A398" sqref="A398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -10721,7 +10758,7 @@
         <v>40</v>
       </c>
       <c r="F383" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="384" spans="1:6" x14ac:dyDescent="0.25">
@@ -10741,7 +10778,7 @@
         <v>90</v>
       </c>
       <c r="F384" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="385" spans="1:6" x14ac:dyDescent="0.25">
@@ -10752,7 +10789,7 @@
         <v>0.62152777777777779</v>
       </c>
       <c r="C385" s="4" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D385" s="2" t="s">
         <v>162</v>
@@ -10761,7 +10798,7 @@
         <v>10</v>
       </c>
       <c r="F385" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="386" spans="1:6" x14ac:dyDescent="0.25">
@@ -10772,7 +10809,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="C386" s="4" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D386" s="2" t="s">
         <v>162</v>
@@ -10781,7 +10818,7 @@
         <v>45</v>
       </c>
       <c r="F386" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="387" spans="1:6" x14ac:dyDescent="0.25">
@@ -10832,7 +10869,7 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="C389" s="4" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D389" s="2" t="s">
         <v>162</v>
@@ -10841,7 +10878,7 @@
         <v>150</v>
       </c>
       <c r="F389" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="390" spans="1:6" x14ac:dyDescent="0.25">
@@ -10861,7 +10898,7 @@
         <v>90</v>
       </c>
       <c r="F390" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.25">
@@ -10881,7 +10918,7 @@
         <v>10</v>
       </c>
       <c r="F391" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.25">
@@ -10892,7 +10929,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="C392" s="4" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D392" s="2" t="s">
         <v>162</v>
@@ -10901,98 +10938,158 @@
         <v>50</v>
       </c>
       <c r="F392" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393" s="5" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B393" s="13">
         <v>0</v>
       </c>
       <c r="C393" s="4" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
       <c r="D393" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E393" s="2"/>
+      <c r="E393" s="2">
+        <v>170</v>
+      </c>
+      <c r="F393" s="1" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="394" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A394" s="5"/>
-      <c r="B394" s="13"/>
+      <c r="A394" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="B394" s="13">
+        <v>0.125</v>
+      </c>
       <c r="C394" s="4" t="s">
-        <v>835</v>
+        <v>856</v>
       </c>
       <c r="D394" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E394" s="2"/>
+      <c r="E394" s="2">
+        <v>60</v>
+      </c>
       <c r="F394" s="1" t="s">
-        <v>836</v>
+        <v>857</v>
       </c>
     </row>
     <row r="395" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A395" s="5"/>
-      <c r="B395" s="13"/>
+      <c r="A395" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="B395" s="13">
+        <v>0.38541666666666669</v>
+      </c>
       <c r="C395" s="4" t="s">
-        <v>838</v>
+        <v>858</v>
       </c>
       <c r="D395" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E395" s="2"/>
+      <c r="E395" s="2">
+        <v>285</v>
+      </c>
+      <c r="F395" s="1" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="396" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A396" s="5"/>
-      <c r="B396" s="13"/>
+      <c r="A396" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="B396" s="13">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="C396" s="4" t="s">
-        <v>837</v>
+        <v>860</v>
       </c>
       <c r="D396" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E396" s="2"/>
+      <c r="E396" s="2">
+        <v>150</v>
+      </c>
+      <c r="F396" s="1" t="s">
+        <v>861</v>
+      </c>
     </row>
     <row r="397" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A397" s="5"/>
-      <c r="B397" s="13"/>
+      <c r="A397" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="B397" s="13">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="C397" s="4" t="s">
-        <v>840</v>
+        <v>862</v>
       </c>
       <c r="D397" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E397" s="2"/>
+      <c r="E397" s="2">
+        <v>215</v>
+      </c>
+      <c r="F397" s="1" t="s">
+        <v>863</v>
+      </c>
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A398" s="5"/>
-      <c r="B398" s="13"/>
+      <c r="A398" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="B398" s="13">
+        <v>3.472222222222222E-3</v>
+      </c>
       <c r="C398" s="4" t="s">
-        <v>841</v>
+        <v>834</v>
       </c>
       <c r="D398" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E398" s="2"/>
+      <c r="E398" s="2">
+        <v>20</v>
+      </c>
+      <c r="F398" s="1" t="s">
+        <v>835</v>
+      </c>
     </row>
     <row r="399" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A399" s="5"/>
-      <c r="B399" s="13"/>
+      <c r="A399" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="B399" s="13">
+        <v>1.7361111111111112E-2</v>
+      </c>
       <c r="C399" s="4" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="D399" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E399" s="2"/>
+      <c r="E399" s="2">
+        <v>115</v>
+      </c>
+      <c r="F399" s="1" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A400" s="5"/>
-      <c r="B400" s="13"/>
+      <c r="A400" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="B400" s="13">
+        <v>9.7222222222222224E-2</v>
+      </c>
       <c r="C400" s="4" t="s">
-        <v>844</v>
+        <v>866</v>
       </c>
       <c r="D400" s="2" t="s">
         <v>162</v>
@@ -11000,49 +11097,78 @@
       <c r="E400" s="2"/>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A401" s="5"/>
-      <c r="B401" s="13"/>
-      <c r="C401" s="4"/>
-      <c r="D401" s="2"/>
+      <c r="A401" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="C401" s="4" t="s">
+        <v>839</v>
+      </c>
+      <c r="D401" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="E401" s="2"/>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A402" s="10"/>
-      <c r="B402" s="10"/>
-      <c r="D402" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E402" s="3">
-        <f>SUM(E2:E401)</f>
-        <v>35570</v>
-      </c>
+      <c r="A402" s="5"/>
+      <c r="B402" s="13"/>
+      <c r="C402" s="4" t="s">
+        <v>840</v>
+      </c>
+      <c r="D402" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E402" s="2"/>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A403" s="10"/>
-      <c r="B403" s="10"/>
-      <c r="D403" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E403" s="3">
-        <f>E402 / 60</f>
-        <v>592.83333333333337</v>
-      </c>
+      <c r="A403" s="5"/>
+      <c r="B403" s="13"/>
+      <c r="C403" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="D403" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E403" s="2"/>
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A404" s="10"/>
-      <c r="B404" s="10"/>
+      <c r="A404" s="5"/>
+      <c r="B404" s="13"/>
+      <c r="C404" s="4" t="s">
+        <v>843</v>
+      </c>
+      <c r="D404" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E404" s="2"/>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A405" s="10"/>
-      <c r="B405" s="10"/>
+      <c r="A405" s="5"/>
+      <c r="B405" s="13"/>
+      <c r="C405" s="4"/>
+      <c r="D405" s="2"/>
+      <c r="E405" s="2"/>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406" s="10"/>
       <c r="B406" s="10"/>
+      <c r="D406" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E406" s="3">
+        <f>SUM(E2:E405)</f>
+        <v>36585</v>
+      </c>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407" s="10"/>
       <c r="B407" s="10"/>
+      <c r="D407" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E407" s="3">
+        <f>E406 / 60</f>
+        <v>609.75</v>
+      </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408" s="10"/>
@@ -12047,6 +12173,22 @@
     <row r="658" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A658" s="10"/>
       <c r="B658" s="10"/>
+    </row>
+    <row r="659" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A659" s="10"/>
+      <c r="B659" s="10"/>
+    </row>
+    <row r="660" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A660" s="10"/>
+      <c r="B660" s="10"/>
+    </row>
+    <row r="661" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A661" s="10"/>
+      <c r="B661" s="10"/>
+    </row>
+    <row r="662" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A662" s="10"/>
+      <c r="B662" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Finalise Compose with Record Controller
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3870" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35313108-6602-4AC5-8A07-BA7BAEFC1411}"/>
+  <xr:revisionPtr revIDLastSave="3963" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD2EF8CE-1BC8-4E6F-829A-5C85F43E4E37}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="886">
   <si>
     <t>Date</t>
   </si>
@@ -2555,15 +2555,6 @@
     <t>Compose - Duration Notation</t>
   </si>
   <si>
-    <t>Compose - Save Tab</t>
-  </si>
-  <si>
-    <t>Compose - Load Tab</t>
-  </si>
-  <si>
-    <t>Compose - Record Guitar Input</t>
-  </si>
-  <si>
     <t>Compose - Note Placement Warning</t>
   </si>
   <si>
@@ -2637,6 +2628,72 @@
   </si>
   <si>
     <t>Compose - Metronome Volume</t>
+  </si>
+  <si>
+    <t>Toggle Metronome</t>
+  </si>
+  <si>
+    <t>Compose - Save Form</t>
+  </si>
+  <si>
+    <t>Create a Save Form with Radio Btns and Slider</t>
+  </si>
+  <si>
+    <t>Compose - Validate Save</t>
+  </si>
+  <si>
+    <t>Complete Save Input Validation</t>
+  </si>
+  <si>
+    <t>Save Guitar Tab</t>
+  </si>
+  <si>
+    <t>Compose - Modify Save (PUT)</t>
+  </si>
+  <si>
+    <t>Modify Guitar Tab when Save Returns Error 409 Conflict and User Has Authority to Do So</t>
+  </si>
+  <si>
+    <t>Compose - Save Tablature (POST)</t>
+  </si>
+  <si>
+    <t>Compose - Load Tabs (GET)</t>
+  </si>
+  <si>
+    <t>Compose - Open Tab Form</t>
+  </si>
+  <si>
+    <t>Create Open Tab Form, Get Items From DB, Public/Private Icons, Difficulty Display, Date, Select Tab from List</t>
+  </si>
+  <si>
+    <t>Get Tab and Validate, Display Loaded Tab</t>
+  </si>
+  <si>
+    <t>Compose - Delete Tabs</t>
+  </si>
+  <si>
+    <t>26.03.2023</t>
+  </si>
+  <si>
+    <t>Compose - Edit Note Debug</t>
+  </si>
+  <si>
+    <t>Note Duration Values are Not Displayed Correctly (Fixed)</t>
+  </si>
+  <si>
+    <t>Clear Tab Sheet If No Saved Tab with User Id and Title Otherwise Delete the Tab From DB and Clear Canvas</t>
+  </si>
+  <si>
+    <t>Compose - Read Guitar Input</t>
+  </si>
+  <si>
+    <t>Read Controller Fret and Position Press and Release Events</t>
+  </si>
+  <si>
+    <t>Compose - Record Guitar</t>
+  </si>
+  <si>
+    <t>Strum Release Start an Unfinalised Note, and Every Other Events Finalise Them, Recalculating Its Duration</t>
   </si>
 </sst>
 </file>
@@ -3077,11 +3134,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M662"/>
+  <dimension ref="A1:M669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A377" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A398" sqref="A398"/>
+      <pane ySplit="1" topLeftCell="A395" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E411" sqref="E411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -10461,7 +10518,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" s="5" t="s">
         <v>784</v>
       </c>
@@ -10481,7 +10538,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A370" s="5" t="s">
         <v>797</v>
       </c>
@@ -10501,7 +10558,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A371" s="5" t="s">
         <v>797</v>
       </c>
@@ -10521,7 +10578,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A372" s="5" t="s">
         <v>797</v>
       </c>
@@ -10541,7 +10598,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A373" s="5" t="s">
         <v>797</v>
       </c>
@@ -10561,7 +10618,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" s="5" t="s">
         <v>805</v>
       </c>
@@ -10581,7 +10638,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A375" s="5" t="s">
         <v>805</v>
       </c>
@@ -10601,7 +10658,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A376" s="5" t="s">
         <v>810</v>
       </c>
@@ -10620,8 +10677,9 @@
       <c r="F376" s="1" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K376" s="2"/>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" s="5" t="s">
         <v>810</v>
       </c>
@@ -10640,8 +10698,9 @@
       <c r="F377" s="1" t="s">
         <v>814</v>
       </c>
-    </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K377" s="2"/>
+    </row>
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378" s="5" t="s">
         <v>810</v>
       </c>
@@ -10660,8 +10719,9 @@
       <c r="F378" s="1" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K378" s="2"/>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" s="5" t="s">
         <v>810</v>
       </c>
@@ -10680,8 +10740,9 @@
       <c r="F379" s="1" t="s">
         <v>821</v>
       </c>
-    </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K379" s="2"/>
+    </row>
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" s="5" t="s">
         <v>819</v>
       </c>
@@ -10700,8 +10761,9 @@
       <c r="F380" s="1" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K380" s="2"/>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A381" s="5" t="s">
         <v>819</v>
       </c>
@@ -10720,8 +10782,9 @@
       <c r="F381" s="1" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K381" s="2"/>
+    </row>
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382" s="5" t="s">
         <v>819</v>
       </c>
@@ -10740,8 +10803,9 @@
       <c r="F382" s="1" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K382" s="2"/>
+    </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A383" s="5" t="s">
         <v>819</v>
       </c>
@@ -10758,10 +10822,11 @@
         <v>40</v>
       </c>
       <c r="F383" s="1" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+        <v>841</v>
+      </c>
+      <c r="K383" s="2"/>
+    </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A384" s="5" t="s">
         <v>819</v>
       </c>
@@ -10778,10 +10843,11 @@
         <v>90</v>
       </c>
       <c r="F384" s="1" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+        <v>842</v>
+      </c>
+      <c r="K384" s="2"/>
+    </row>
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A385" s="5" t="s">
         <v>819</v>
       </c>
@@ -10789,7 +10855,7 @@
         <v>0.62152777777777779</v>
       </c>
       <c r="C385" s="4" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="D385" s="2" t="s">
         <v>162</v>
@@ -10798,10 +10864,11 @@
         <v>10</v>
       </c>
       <c r="F385" s="1" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+        <v>843</v>
+      </c>
+      <c r="K385" s="2"/>
+    </row>
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A386" s="5" t="s">
         <v>819</v>
       </c>
@@ -10809,7 +10876,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="C386" s="4" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="D386" s="2" t="s">
         <v>162</v>
@@ -10818,10 +10885,11 @@
         <v>45</v>
       </c>
       <c r="F386" s="1" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+        <v>845</v>
+      </c>
+      <c r="K386" s="2"/>
+    </row>
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A387" s="5" t="s">
         <v>819</v>
       </c>
@@ -10840,8 +10908,9 @@
       <c r="F387" s="1" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K387" s="2"/>
+    </row>
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A388" s="5" t="s">
         <v>819</v>
       </c>
@@ -10860,8 +10929,9 @@
       <c r="F388" s="1" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K388" s="2"/>
+    </row>
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A389" s="5" t="s">
         <v>819</v>
       </c>
@@ -10878,10 +10948,11 @@
         <v>150</v>
       </c>
       <c r="F389" s="1" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+        <v>846</v>
+      </c>
+      <c r="K389" s="2"/>
+    </row>
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A390" s="5" t="s">
         <v>819</v>
       </c>
@@ -10898,10 +10969,11 @@
         <v>90</v>
       </c>
       <c r="F390" s="1" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+        <v>847</v>
+      </c>
+      <c r="K390" s="2"/>
+    </row>
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" s="5" t="s">
         <v>819</v>
       </c>
@@ -10918,10 +10990,11 @@
         <v>10</v>
       </c>
       <c r="F391" s="1" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+        <v>848</v>
+      </c>
+      <c r="K391" s="2"/>
+    </row>
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A392" s="5" t="s">
         <v>819</v>
       </c>
@@ -10929,7 +11002,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="C392" s="4" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="D392" s="2" t="s">
         <v>162</v>
@@ -10938,12 +11011,13 @@
         <v>50</v>
       </c>
       <c r="F392" s="1" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+        <v>851</v>
+      </c>
+      <c r="K392" s="2"/>
+    </row>
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A393" s="5" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="B393" s="13">
         <v>0</v>
@@ -10958,18 +11032,19 @@
         <v>170</v>
       </c>
       <c r="F393" s="1" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+        <v>852</v>
+      </c>
+      <c r="K393" s="2"/>
+    </row>
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A394" s="5" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="B394" s="13">
         <v>0.125</v>
       </c>
       <c r="C394" s="4" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="D394" s="2" t="s">
         <v>162</v>
@@ -10978,18 +11053,19 @@
         <v>60</v>
       </c>
       <c r="F394" s="1" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+        <v>854</v>
+      </c>
+      <c r="K394" s="2"/>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A395" s="5" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="B395" s="13">
         <v>0.38541666666666669</v>
       </c>
       <c r="C395" s="4" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="D395" s="2" t="s">
         <v>162</v>
@@ -10998,18 +11074,19 @@
         <v>285</v>
       </c>
       <c r="F395" s="1" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+        <v>856</v>
+      </c>
+      <c r="K395" s="2"/>
+    </row>
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" s="5" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="B396" s="13">
         <v>0.70833333333333337</v>
       </c>
       <c r="C396" s="4" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="D396" s="2" t="s">
         <v>162</v>
@@ -11018,18 +11095,19 @@
         <v>150</v>
       </c>
       <c r="F396" s="1" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+        <v>858</v>
+      </c>
+      <c r="K396" s="2"/>
+    </row>
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" s="5" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="B397" s="13">
         <v>0.83333333333333337</v>
       </c>
       <c r="C397" s="4" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="D397" s="2" t="s">
         <v>162</v>
@@ -11038,12 +11116,13 @@
         <v>215</v>
       </c>
       <c r="F397" s="1" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+        <v>860</v>
+      </c>
+      <c r="K397" s="2"/>
+    </row>
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A398" s="5" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="B398" s="13">
         <v>3.472222222222222E-3</v>
@@ -11060,10 +11139,11 @@
       <c r="F398" s="1" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K398" s="2"/>
+    </row>
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A399" s="5" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="B399" s="13">
         <v>1.7361111111111112E-2</v>
@@ -11078,131 +11158,280 @@
         <v>115</v>
       </c>
       <c r="F399" s="1" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+        <v>862</v>
+      </c>
+      <c r="K399" s="2"/>
+    </row>
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A400" s="5" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="B400" s="13">
         <v>9.7222222222222224E-2</v>
       </c>
       <c r="C400" s="4" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="D400" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E400" s="2"/>
-    </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E400" s="2">
+        <v>15</v>
+      </c>
+      <c r="F400" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="K400" s="2"/>
+    </row>
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A401" s="5" t="s">
-        <v>864</v>
+        <v>861</v>
+      </c>
+      <c r="B401" s="13">
+        <v>0.1076388888888889</v>
       </c>
       <c r="C401" s="4" t="s">
-        <v>839</v>
+        <v>865</v>
       </c>
       <c r="D401" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E401" s="2"/>
-    </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A402" s="5"/>
-      <c r="B402" s="13"/>
+      <c r="E401" s="2">
+        <v>110</v>
+      </c>
+      <c r="F401" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="K401" s="2"/>
+    </row>
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A402" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="B402" s="13">
+        <v>0.18055555555555555</v>
+      </c>
       <c r="C402" s="4" t="s">
-        <v>840</v>
+        <v>867</v>
       </c>
       <c r="D402" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E402" s="2"/>
-    </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A403" s="5"/>
-      <c r="B403" s="13"/>
+      <c r="E402" s="2">
+        <v>40</v>
+      </c>
+      <c r="F402" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="K402" s="2"/>
+    </row>
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A403" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="B403" s="13">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="C403" s="4" t="s">
-        <v>841</v>
+        <v>872</v>
       </c>
       <c r="D403" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E403" s="2"/>
-    </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A404" s="5"/>
-      <c r="B404" s="13"/>
+      <c r="E403" s="2">
+        <v>15</v>
+      </c>
+      <c r="F403" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="K403" s="2"/>
+    </row>
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A404" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="B404" s="13">
+        <v>0.625</v>
+      </c>
       <c r="C404" s="4" t="s">
-        <v>843</v>
+        <v>870</v>
       </c>
       <c r="D404" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E404" s="2"/>
-    </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A405" s="5"/>
-      <c r="B405" s="13"/>
-      <c r="C405" s="4"/>
-      <c r="D405" s="2"/>
-      <c r="E405" s="2"/>
-    </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A406" s="10"/>
-      <c r="B406" s="10"/>
-      <c r="D406" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E406" s="3">
-        <f>SUM(E2:E405)</f>
-        <v>36585</v>
-      </c>
-    </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A407" s="10"/>
-      <c r="B407" s="10"/>
-      <c r="D407" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E407" s="3">
-        <f>E406 / 60</f>
-        <v>609.75</v>
-      </c>
-    </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A408" s="10"/>
-      <c r="B408" s="10"/>
-    </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A409" s="10"/>
-      <c r="B409" s="10"/>
-    </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A410" s="10"/>
-      <c r="B410" s="10"/>
-    </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A411" s="10"/>
-      <c r="B411" s="10"/>
-    </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A412" s="10"/>
-      <c r="B412" s="10"/>
-    </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E404" s="2">
+        <v>70</v>
+      </c>
+      <c r="F404" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="K404" s="2"/>
+    </row>
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A405" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="B405" s="13">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="C405" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="D405" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E405" s="2">
+        <v>165</v>
+      </c>
+      <c r="F405" s="1" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A406" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="B406" s="13">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="C406" s="4" t="s">
+        <v>873</v>
+      </c>
+      <c r="D406" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E406" s="2">
+        <v>135</v>
+      </c>
+      <c r="F406" s="1" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A407" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="B407" s="13">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C407" s="4" t="s">
+        <v>879</v>
+      </c>
+      <c r="D407" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E407" s="2">
+        <v>30</v>
+      </c>
+      <c r="F407" s="1" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A408" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="B408" s="13">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C408" s="4" t="s">
+        <v>877</v>
+      </c>
+      <c r="D408" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E408" s="2">
+        <v>90</v>
+      </c>
+      <c r="F408" s="1" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A409" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="B409" s="13">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="C409" s="4" t="s">
+        <v>882</v>
+      </c>
+      <c r="D409" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E409" s="2">
+        <v>40</v>
+      </c>
+      <c r="F409" s="1" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A410" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="B410" s="13">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="C410" s="4" t="s">
+        <v>884</v>
+      </c>
+      <c r="D410" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E410" s="2">
+        <v>445</v>
+      </c>
+      <c r="F410" s="1" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A411" s="5"/>
+      <c r="B411" s="13"/>
+      <c r="C411" s="4" t="s">
+        <v>840</v>
+      </c>
+      <c r="D411" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E411" s="2"/>
+    </row>
+    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A412" s="5"/>
+      <c r="B412" s="13"/>
+      <c r="C412" s="4"/>
+      <c r="D412" s="2"/>
+      <c r="E412" s="2"/>
+    </row>
+    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A413" s="10"/>
       <c r="B413" s="10"/>
-    </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D413" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E413" s="3">
+        <f>SUM(E2:E412)</f>
+        <v>37740</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A414" s="10"/>
       <c r="B414" s="10"/>
-    </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D414" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E414" s="3">
+        <f>E413 / 60</f>
+        <v>629</v>
+      </c>
+    </row>
+    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A415" s="10"/>
       <c r="B415" s="10"/>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A416" s="10"/>
       <c r="B416" s="10"/>
     </row>
@@ -12189,6 +12418,34 @@
     <row r="662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A662" s="10"/>
       <c r="B662" s="10"/>
+    </row>
+    <row r="663" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A663" s="10"/>
+      <c r="B663" s="10"/>
+    </row>
+    <row r="664" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A664" s="10"/>
+      <c r="B664" s="10"/>
+    </row>
+    <row r="665" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A665" s="10"/>
+      <c r="B665" s="10"/>
+    </row>
+    <row r="666" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A666" s="10"/>
+      <c r="B666" s="10"/>
+    </row>
+    <row r="667" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A667" s="10"/>
+      <c r="B667" s="10"/>
+    </row>
+    <row r="668" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A668" s="10"/>
+      <c r="B668" s="10"/>
+    </row>
+    <row r="669" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A669" s="10"/>
+      <c r="B669" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Start Practice Page and Note Track
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3963" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD2EF8CE-1BC8-4E6F-829A-5C85F43E4E37}"/>
+  <xr:revisionPtr revIDLastSave="4118" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{321D0805-F45A-4472-A769-9B3D65251E2E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="925">
   <si>
     <t>Date</t>
   </si>
@@ -2694,6 +2694,123 @@
   </si>
   <si>
     <t>Strum Release Start an Unfinalised Note, and Every Other Events Finalise Them, Recalculating Its Duration</t>
+  </si>
+  <si>
+    <t>19.04.2023</t>
+  </si>
+  <si>
+    <t>Fetch Avatar and Name from Db and Display on Homepage</t>
+  </si>
+  <si>
+    <t>18.04.2023</t>
+  </si>
+  <si>
+    <t>16.04.2023</t>
+  </si>
+  <si>
+    <t>Edit Higher E Note Always Displays Undefined (Solved: Misspelled Object Properte was Loaded into Memory)</t>
+  </si>
+  <si>
+    <t>29.03.2023</t>
+  </si>
+  <si>
+    <t>Produce Tab Metallica: Master of Puppets Intro</t>
+  </si>
+  <si>
+    <t>30.03.2023</t>
+  </si>
+  <si>
+    <t>Produce Tabs 1</t>
+  </si>
+  <si>
+    <t>Produce Tabs 2</t>
+  </si>
+  <si>
+    <t>Produce Tabs 3</t>
+  </si>
+  <si>
+    <t>Produce Tabs 4</t>
+  </si>
+  <si>
+    <t>Produce Tab Madonna: Secret (Needs More Polishing)</t>
+  </si>
+  <si>
+    <t>Produce Tab Metallica: Nothing Else Matters Intro</t>
+  </si>
+  <si>
+    <t>Produce Tab Bikini: Kozeli Helyeken Part 1</t>
+  </si>
+  <si>
+    <t>Compose - Debug 1</t>
+  </si>
+  <si>
+    <t>Compose - Debug 2</t>
+  </si>
+  <si>
+    <t>04.04.2023</t>
+  </si>
+  <si>
+    <t>06.04.2023</t>
+  </si>
+  <si>
+    <t>When Recording Guitar, Quick Multi-String Strums Produce Undefined for Chordname and Notes are Cut Short (Might Lead Back to String Debouncing)</t>
+  </si>
+  <si>
+    <t>Debounce Control</t>
+  </si>
+  <si>
+    <t>Create a Debounce Control, If Strum or Fret Activated and Deactivated to Fast, Do Not Register Message (Works But Sometimes Skips)</t>
+  </si>
+  <si>
+    <t>Revise Debounce Control</t>
+  </si>
+  <si>
+    <t>Break Down the Switch State Issue: Two Separate Debounce Compensation for Strims and Frets</t>
+  </si>
+  <si>
+    <t>Document Debounce</t>
+  </si>
+  <si>
+    <t>Diagram of Fret and Strumn Debounce and Explanation and Code Snippets</t>
+  </si>
+  <si>
+    <t>19.05.2023</t>
+  </si>
+  <si>
+    <t>20.05.2023</t>
+  </si>
+  <si>
+    <t>Practice - Basic Structure</t>
+  </si>
+  <si>
+    <t>The Fundamental Structure of the Page Header, Tab, Track, Guitar, Footer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make Page Show Guitar Comnponent and Read Values of Controller </t>
+  </si>
+  <si>
+    <t>Practice - Integrate Tab Sheet</t>
+  </si>
+  <si>
+    <t>Tab is Displayed, Can be Played, Paused and Stopped</t>
+  </si>
+  <si>
+    <t>21.05.2023</t>
+  </si>
+  <si>
+    <t>Practice - Integrate Guitar</t>
+  </si>
+  <si>
+    <t>Practice - Create Note Track 1</t>
+  </si>
+  <si>
+    <t>Practice - Create Note Track 2</t>
+  </si>
+  <si>
+    <t>Create Physical Strings and a Predefined Number of Prev and Next Beat</t>
+  </si>
+  <si>
+    <t>Transform Bars Into A Less Expensive Format that is More Performant for This Scenario</t>
   </si>
 </sst>
 </file>
@@ -3134,11 +3251,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M669"/>
+  <dimension ref="A1:M685"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A395" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E411" sqref="E411"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A412" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F425" sqref="F425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -11388,114 +11505,353 @@
       </c>
     </row>
     <row r="411" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A411" s="5"/>
-      <c r="B411" s="13"/>
+      <c r="A411" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="B411" s="13">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="C411" s="4" t="s">
+        <v>894</v>
+      </c>
+      <c r="D411" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E411" s="2">
+        <v>25</v>
+      </c>
+      <c r="F411" s="1" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A412" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="B412" s="13">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="C412" s="4" t="s">
+        <v>895</v>
+      </c>
+      <c r="D412" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E412" s="2">
+        <v>40</v>
+      </c>
+      <c r="F412" s="1" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A413" s="5" t="s">
+        <v>903</v>
+      </c>
+      <c r="B413" s="13">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="C413" s="4" t="s">
+        <v>896</v>
+      </c>
+      <c r="D413" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E413" s="2">
+        <v>15</v>
+      </c>
+      <c r="F413" s="1" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A414" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="B414" s="13">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="C414" s="4" t="s">
+        <v>897</v>
+      </c>
+      <c r="D414" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E414" s="2">
+        <v>35</v>
+      </c>
+      <c r="F414" s="1" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A415" s="5" t="s">
+        <v>889</v>
+      </c>
+      <c r="B415" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C415" s="4" t="s">
+        <v>901</v>
+      </c>
+      <c r="D415" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E415" s="2">
+        <v>20</v>
+      </c>
+      <c r="F415" s="1" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A416" s="5" t="s">
+        <v>888</v>
+      </c>
+      <c r="B416" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C416" s="4" t="s">
         <v>840</v>
       </c>
-      <c r="D411" s="2" t="s">
+      <c r="D416" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E411" s="2"/>
-    </row>
-    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A412" s="5"/>
-      <c r="B412" s="13"/>
-      <c r="C412" s="4"/>
-      <c r="D412" s="2"/>
-      <c r="E412" s="2"/>
-    </row>
-    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A413" s="10"/>
-      <c r="B413" s="10"/>
-      <c r="D413" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E413" s="3">
-        <f>SUM(E2:E412)</f>
-        <v>37740</v>
-      </c>
-    </row>
-    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A414" s="10"/>
-      <c r="B414" s="10"/>
-      <c r="D414" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E414" s="3">
-        <f>E413 / 60</f>
-        <v>629</v>
-      </c>
-    </row>
-    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A415" s="10"/>
-      <c r="B415" s="10"/>
-    </row>
-    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A416" s="10"/>
-      <c r="B416" s="10"/>
-    </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A417" s="10"/>
-      <c r="B417" s="10"/>
-    </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A418" s="10"/>
-      <c r="B418" s="10"/>
-    </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A419" s="10"/>
-      <c r="B419" s="10"/>
-    </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A420" s="10"/>
-      <c r="B420" s="10"/>
-    </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A421" s="10"/>
-      <c r="B421" s="10"/>
-    </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A422" s="10"/>
-      <c r="B422" s="10"/>
-    </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A423" s="10"/>
-      <c r="B423" s="10"/>
-    </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A424" s="10"/>
-      <c r="B424" s="10"/>
-    </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A425" s="10"/>
-      <c r="B425" s="10"/>
-    </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A426" s="10"/>
-      <c r="B426" s="10"/>
-    </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A427" s="10"/>
-      <c r="B427" s="10"/>
-    </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A428" s="10"/>
-      <c r="B428" s="10"/>
-    </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E416" s="2">
+        <v>65</v>
+      </c>
+      <c r="F416" s="1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A417" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="B417" s="13">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="C417" s="4" t="s">
+        <v>902</v>
+      </c>
+      <c r="D417" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E417" s="2">
+        <v>55</v>
+      </c>
+      <c r="F417" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A418" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="B418" s="13">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="C418" s="4" t="s">
+        <v>906</v>
+      </c>
+      <c r="D418" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E418" s="2">
+        <v>125</v>
+      </c>
+      <c r="F418" s="1" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A419" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="B419" s="13">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C419" s="4" t="s">
+        <v>908</v>
+      </c>
+      <c r="D419" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E419" s="2">
+        <v>195</v>
+      </c>
+      <c r="F419" s="1" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A420" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="B420" s="13">
+        <v>9.375E-2</v>
+      </c>
+      <c r="C420" s="4" t="s">
+        <v>910</v>
+      </c>
+      <c r="D420" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E420" s="2">
+        <v>45</v>
+      </c>
+      <c r="F420" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A421" s="5" t="s">
+        <v>913</v>
+      </c>
+      <c r="B421" s="13">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="C421" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="D421" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E421" s="2">
+        <v>20</v>
+      </c>
+      <c r="F421" s="1" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A422" s="5" t="s">
+        <v>913</v>
+      </c>
+      <c r="B422" s="13">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C422" s="4" t="s">
+        <v>920</v>
+      </c>
+      <c r="D422" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E422" s="2">
+        <v>40</v>
+      </c>
+      <c r="F422" s="1" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A423" s="5" t="s">
+        <v>913</v>
+      </c>
+      <c r="B423" s="13">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C423" s="4" t="s">
+        <v>917</v>
+      </c>
+      <c r="D423" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E423" s="2">
+        <v>170</v>
+      </c>
+      <c r="F423" s="1" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A424" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="B424" s="13">
+        <v>0.11805555555555557</v>
+      </c>
+      <c r="C424" s="4" t="s">
+        <v>921</v>
+      </c>
+      <c r="D424" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E424" s="2">
+        <v>30</v>
+      </c>
+      <c r="F424" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A425" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="B425" s="13">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="C425" s="4" t="s">
+        <v>922</v>
+      </c>
+      <c r="D425" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E425" s="2">
+        <v>120</v>
+      </c>
+      <c r="F425" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A426" s="5"/>
+      <c r="B426" s="13"/>
+      <c r="C426" s="4"/>
+      <c r="D426" s="2"/>
+      <c r="E426" s="2"/>
+    </row>
+    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A427" s="5"/>
+      <c r="B427" s="13"/>
+      <c r="C427" s="4"/>
+      <c r="D427" s="2"/>
+      <c r="E427" s="2"/>
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A428" s="5"/>
+      <c r="B428" s="13"/>
+      <c r="C428" s="4"/>
+      <c r="D428" s="2"/>
+      <c r="E428" s="2"/>
+    </row>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A429" s="10"/>
       <c r="B429" s="10"/>
-    </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D429" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E429" s="3">
+        <f>SUM(E2:E425)</f>
+        <v>38740</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A430" s="10"/>
       <c r="B430" s="10"/>
-    </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D430" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E430" s="3">
+        <f>E429 / 60</f>
+        <v>645.66666666666663</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A431" s="10"/>
       <c r="B431" s="10"/>
     </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A432" s="10"/>
       <c r="B432" s="10"/>
     </row>
@@ -12446,6 +12802,70 @@
     <row r="669" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A669" s="10"/>
       <c r="B669" s="10"/>
+    </row>
+    <row r="670" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A670" s="10"/>
+      <c r="B670" s="10"/>
+    </row>
+    <row r="671" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A671" s="10"/>
+      <c r="B671" s="10"/>
+    </row>
+    <row r="672" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A672" s="10"/>
+      <c r="B672" s="10"/>
+    </row>
+    <row r="673" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A673" s="10"/>
+      <c r="B673" s="10"/>
+    </row>
+    <row r="674" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A674" s="10"/>
+      <c r="B674" s="10"/>
+    </row>
+    <row r="675" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A675" s="10"/>
+      <c r="B675" s="10"/>
+    </row>
+    <row r="676" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A676" s="10"/>
+      <c r="B676" s="10"/>
+    </row>
+    <row r="677" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A677" s="10"/>
+      <c r="B677" s="10"/>
+    </row>
+    <row r="678" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A678" s="10"/>
+      <c r="B678" s="10"/>
+    </row>
+    <row r="679" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A679" s="10"/>
+      <c r="B679" s="10"/>
+    </row>
+    <row r="680" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A680" s="10"/>
+      <c r="B680" s="10"/>
+    </row>
+    <row r="681" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A681" s="10"/>
+      <c r="B681" s="10"/>
+    </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A682" s="10"/>
+      <c r="B682" s="10"/>
+    </row>
+    <row r="683" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A683" s="10"/>
+      <c r="B683" s="10"/>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A684" s="10"/>
+      <c r="B684" s="10"/>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A685" s="10"/>
+      <c r="B685" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Note Track Works Accordingly: Refreshes Accurately for Bar and Note Index Changes
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4118" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{321D0805-F45A-4472-A769-9B3D65251E2E}"/>
+  <xr:revisionPtr revIDLastSave="4123" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A15A94CC-32AE-4130-91AE-D3EEDDB2C8E5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="927">
   <si>
     <t>Date</t>
   </si>
@@ -2811,6 +2811,12 @@
   </si>
   <si>
     <t>Transform Bars Into A Less Expensive Format that is More Performant for This Scenario</t>
+  </si>
+  <si>
+    <t>Practice - Create Note Track 3</t>
+  </si>
+  <si>
+    <t>Fill Up Note Track with Bar Values</t>
   </si>
 </sst>
 </file>
@@ -3255,7 +3261,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A412" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F425" sqref="F425"/>
+      <selection pane="bottomLeft" activeCell="E426" sqref="E426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -11805,11 +11811,22 @@
       </c>
     </row>
     <row r="426" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A426" s="5"/>
-      <c r="B426" s="13"/>
-      <c r="C426" s="4"/>
-      <c r="D426" s="2"/>
+      <c r="A426" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="B426" s="13">
+        <v>0.6875</v>
+      </c>
+      <c r="C426" s="4" t="s">
+        <v>925</v>
+      </c>
+      <c r="D426" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="E426" s="2"/>
+      <c r="F426" s="1" t="s">
+        <v>926</v>
+      </c>
     </row>
     <row r="427" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A427" s="5"/>

</xml_diff>

<commit_message>
Finish Practice and Play Options
</commit_message>
<xml_diff>
--- a/Documentation/Project Log Book.xlsx
+++ b/Documentation/Project Log Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5849fbde5c4cf694/Desktop/Uni/Uni Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4123" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A15A94CC-32AE-4130-91AE-D3EEDDB2C8E5}"/>
+  <xr:revisionPtr revIDLastSave="4316" documentId="8_{000771A0-308D-4BFA-96AA-02BC4AC14DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5664D893-F5CF-4089-9A87-631D8FA35FE0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43229390-D9E6-4EBD-A715-EF6E60A7C3EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="976">
   <si>
     <t>Date</t>
   </si>
@@ -2817,6 +2817,153 @@
   </si>
   <si>
     <t>Fill Up Note Track with Bar Values</t>
+  </si>
+  <si>
+    <t>23.05.2023</t>
+  </si>
+  <si>
+    <t>Practice - Play Track</t>
+  </si>
+  <si>
+    <t>Note Track Only Updates On Bar Index Changes (Needs Debugging)</t>
+  </si>
+  <si>
+    <t>24.05.2023</t>
+  </si>
+  <si>
+    <t>Practice - Track Debugging</t>
+  </si>
+  <si>
+    <t>Rewrite How Positions are Calculated, Including Accounting for Note Index Changes (Fixed)</t>
+  </si>
+  <si>
+    <t>27.05.2023</t>
+  </si>
+  <si>
+    <t>Practice - Count Down</t>
+  </si>
+  <si>
+    <t>Create a Stylised Cound Down Every Time Play Pressed</t>
+  </si>
+  <si>
+    <t>Practice - Play Audio</t>
+  </si>
+  <si>
+    <t>Edit Sample Audio File and Play, Pause and Stop Audio with Track</t>
+  </si>
+  <si>
+    <t>Practice - Synchronise Audio</t>
+  </si>
+  <si>
+    <t>Make Tab Play Together with Audio at the Same Exact Pace</t>
+  </si>
+  <si>
+    <t>Produce Tabs 5</t>
+  </si>
+  <si>
+    <t>Finish Metallica Nothing Else Matters Intro</t>
+  </si>
+  <si>
+    <t>Practice - Register Strums</t>
+  </si>
+  <si>
+    <t>Register Each Strum that the Controller Device Make for Each String</t>
+  </si>
+  <si>
+    <t>Practice - Accuracy</t>
+  </si>
+  <si>
+    <t>Compare Each Current Beat to the Actual Guitar Strums</t>
+  </si>
+  <si>
+    <t>Software Intro Paragraph</t>
+  </si>
+  <si>
+    <t>Short Intro for Software Development Paragraph</t>
+  </si>
+  <si>
+    <t>Materials Paragraph</t>
+  </si>
+  <si>
+    <t>Write About Audio Cutting and Other Sources</t>
+  </si>
+  <si>
+    <t>28.05.2023</t>
+  </si>
+  <si>
+    <t>Chords and Avatars Paragraph</t>
+  </si>
+  <si>
+    <t>Document Chord List JSON and Avatar Creation</t>
+  </si>
+  <si>
+    <t>Digital Design</t>
+  </si>
+  <si>
+    <t>Some Code Snippets and Explanation plus Snapshot of Neumorphic Elements</t>
+  </si>
+  <si>
+    <t>Document Registration Page</t>
+  </si>
+  <si>
+    <t>Document Proile Page</t>
+  </si>
+  <si>
+    <t>Snapshot and Explanation</t>
+  </si>
+  <si>
+    <t>Snapshot, Code Snippet from Auto Completion and Explanation</t>
+  </si>
+  <si>
+    <t>Document Landing Page</t>
+  </si>
+  <si>
+    <t>Snapshot, Code Snippet about Asyc Await and Explanation</t>
+  </si>
+  <si>
+    <t>Document Jam Session</t>
+  </si>
+  <si>
+    <t>Snapshot, Explanation of Guitar Neck Board and Equaliser, Timers etc</t>
+  </si>
+  <si>
+    <t>Document Chord Page</t>
+  </si>
+  <si>
+    <t>Filtering, Diagram, Card Generation</t>
+  </si>
+  <si>
+    <t>Document Compose 1</t>
+  </si>
+  <si>
+    <t>Basic Intro of Features</t>
+  </si>
+  <si>
+    <t>29.05.2023</t>
+  </si>
+  <si>
+    <t>Practice - Accuracy 2</t>
+  </si>
+  <si>
+    <t>Read Precision: Every Strum Looks Ahead and Behind for 10 Beats to Find Start Position and Calculates Precision</t>
+  </si>
+  <si>
+    <t>Practice - Header</t>
+  </si>
+  <si>
+    <t>Display Score Title and Score Results</t>
+  </si>
+  <si>
+    <t>Play - Basics</t>
+  </si>
+  <si>
+    <t>Copy All Existing Practice Functionalities to Play and create Play Model</t>
+  </si>
+  <si>
+    <t>Play - POST, GET All, Get ID</t>
+  </si>
+  <si>
+    <t>Save Score After a Play</t>
   </si>
 </sst>
 </file>
@@ -3257,11 +3404,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B349D5-7FEC-4BA2-A4F4-AEC45E6B72AD}">
-  <dimension ref="A1:M685"/>
+  <dimension ref="A1:M708"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A412" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E426" sqref="E426"/>
+      <pane ySplit="1" topLeftCell="A421" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F448" sqref="F448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -11823,180 +11970,537 @@
       <c r="D426" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E426" s="2"/>
+      <c r="E426" s="2">
+        <v>90</v>
+      </c>
       <c r="F426" s="1" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="427" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A427" s="5"/>
-      <c r="B427" s="13"/>
-      <c r="C427" s="4"/>
-      <c r="D427" s="2"/>
-      <c r="E427" s="2"/>
+      <c r="A427" s="5" t="s">
+        <v>927</v>
+      </c>
+      <c r="B427" s="13">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C427" s="4" t="s">
+        <v>928</v>
+      </c>
+      <c r="D427" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E427" s="2">
+        <v>75</v>
+      </c>
+      <c r="F427" s="1" t="s">
+        <v>929</v>
+      </c>
     </row>
     <row r="428" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A428" s="5"/>
-      <c r="B428" s="13"/>
-      <c r="C428" s="4"/>
-      <c r="D428" s="2"/>
-      <c r="E428" s="2"/>
+      <c r="A428" s="5" t="s">
+        <v>930</v>
+      </c>
+      <c r="B428" s="13">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="C428" s="4" t="s">
+        <v>931</v>
+      </c>
+      <c r="D428" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E428" s="2">
+        <v>40</v>
+      </c>
+      <c r="F428" s="1" t="s">
+        <v>932</v>
+      </c>
     </row>
     <row r="429" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A429" s="10"/>
-      <c r="B429" s="10"/>
-      <c r="D429" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E429" s="3">
-        <f>SUM(E2:E425)</f>
-        <v>38740</v>
+      <c r="A429" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="B429" s="13">
+        <v>0.5625</v>
+      </c>
+      <c r="C429" s="4" t="s">
+        <v>934</v>
+      </c>
+      <c r="D429" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E429" s="2">
+        <v>75</v>
+      </c>
+      <c r="F429" s="1" t="s">
+        <v>935</v>
       </c>
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A430" s="10"/>
-      <c r="B430" s="10"/>
-      <c r="D430" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E430" s="3">
-        <f>E429 / 60</f>
-        <v>645.66666666666663</v>
+      <c r="A430" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="B430" s="13">
+        <v>0.65625</v>
+      </c>
+      <c r="C430" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="D430" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E430" s="2">
+        <v>45</v>
+      </c>
+      <c r="F430" s="1" t="s">
+        <v>937</v>
       </c>
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A431" s="10"/>
-      <c r="B431" s="10"/>
+      <c r="A431" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="B431" s="13">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="C431" s="4" t="s">
+        <v>938</v>
+      </c>
+      <c r="D431" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E431" s="2">
+        <v>20</v>
+      </c>
+      <c r="F431" s="1" t="s">
+        <v>939</v>
+      </c>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A432" s="10"/>
-      <c r="B432" s="10"/>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A433" s="10"/>
-      <c r="B433" s="10"/>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A434" s="10"/>
-      <c r="B434" s="10"/>
-    </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A435" s="10"/>
-      <c r="B435" s="10"/>
-    </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A436" s="10"/>
-      <c r="B436" s="10"/>
-    </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A437" s="10"/>
-      <c r="B437" s="10"/>
-    </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A438" s="10"/>
-      <c r="B438" s="10"/>
-    </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A439" s="10"/>
-      <c r="B439" s="10"/>
-    </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A440" s="10"/>
-      <c r="B440" s="10"/>
-    </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A441" s="10"/>
-      <c r="B441" s="10"/>
-    </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A442" s="10"/>
-      <c r="B442" s="10"/>
-    </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A443" s="10"/>
-      <c r="B443" s="10"/>
-    </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A444" s="10"/>
-      <c r="B444" s="10"/>
-    </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A445" s="10"/>
-      <c r="B445" s="10"/>
-    </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A446" s="10"/>
-      <c r="B446" s="10"/>
-    </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A447" s="10"/>
-      <c r="B447" s="10"/>
-    </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A448" s="10"/>
-      <c r="B448" s="10"/>
-    </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A449" s="10"/>
-      <c r="B449" s="10"/>
-    </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A450" s="10"/>
-      <c r="B450" s="10"/>
-    </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A451" s="10"/>
-      <c r="B451" s="10"/>
-    </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="B432" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C432" s="4" t="s">
+        <v>940</v>
+      </c>
+      <c r="D432" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E432" s="2">
+        <v>120</v>
+      </c>
+      <c r="F432" s="1" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A433" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="B433" s="13">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="C433" s="4" t="s">
+        <v>942</v>
+      </c>
+      <c r="D433" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E433" s="2">
+        <v>65</v>
+      </c>
+      <c r="F433" s="1" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A434" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="B434" s="13">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="C434" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="D434" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E434" s="2">
+        <v>40</v>
+      </c>
+      <c r="F434" s="1" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A435" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="B435" s="13">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C435" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="D435" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E435" s="2">
+        <v>30</v>
+      </c>
+      <c r="F435" s="1" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A436" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="B436" s="13">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="C436" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D436" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E436" s="2">
+        <v>35</v>
+      </c>
+      <c r="F436" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A437" s="5" t="s">
+        <v>950</v>
+      </c>
+      <c r="B437" s="13">
+        <v>0</v>
+      </c>
+      <c r="C437" s="4" t="s">
+        <v>951</v>
+      </c>
+      <c r="D437" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E437" s="2">
+        <v>35</v>
+      </c>
+      <c r="F437" s="1" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A438" s="5" t="s">
+        <v>950</v>
+      </c>
+      <c r="B438" s="13">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="C438" s="4" t="s">
+        <v>953</v>
+      </c>
+      <c r="D438" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E438" s="2">
+        <v>25</v>
+      </c>
+      <c r="F438" s="1" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A439" s="5" t="s">
+        <v>950</v>
+      </c>
+      <c r="B439" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C439" s="4" t="s">
+        <v>955</v>
+      </c>
+      <c r="D439" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E439" s="2">
+        <v>25</v>
+      </c>
+      <c r="F439" s="1" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A440" s="5" t="s">
+        <v>950</v>
+      </c>
+      <c r="B440" s="13">
+        <v>5.9027777777777783E-2</v>
+      </c>
+      <c r="C440" s="4" t="s">
+        <v>956</v>
+      </c>
+      <c r="D440" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E440" s="2">
+        <v>35</v>
+      </c>
+      <c r="F440" s="1" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A441" s="5" t="s">
+        <v>950</v>
+      </c>
+      <c r="B441" s="13">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C441" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="D441" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E441" s="2">
+        <v>30</v>
+      </c>
+      <c r="F441" s="1" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A442" s="5" t="s">
+        <v>950</v>
+      </c>
+      <c r="B442" s="13">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C442" s="4" t="s">
+        <v>961</v>
+      </c>
+      <c r="D442" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E442" s="2">
+        <v>35</v>
+      </c>
+      <c r="F442" s="1" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A443" s="5" t="s">
+        <v>950</v>
+      </c>
+      <c r="B443" s="13">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="C443" s="4" t="s">
+        <v>963</v>
+      </c>
+      <c r="D443" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E443" s="2">
+        <v>120</v>
+      </c>
+      <c r="F443" s="1" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A444" s="5" t="s">
+        <v>950</v>
+      </c>
+      <c r="B444" s="13">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="C444" s="4" t="s">
+        <v>965</v>
+      </c>
+      <c r="D444" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E444" s="2">
+        <v>40</v>
+      </c>
+      <c r="F444" s="1" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A445" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B445" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="C445" s="4" t="s">
+        <v>968</v>
+      </c>
+      <c r="D445" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E445" s="2">
+        <v>110</v>
+      </c>
+      <c r="F445" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A446" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B446" s="13">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="C446" s="4" t="s">
+        <v>970</v>
+      </c>
+      <c r="D446" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E446" s="2">
+        <v>90</v>
+      </c>
+      <c r="F446" s="1" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A447" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B447" s="13">
+        <v>0.75694444444444453</v>
+      </c>
+      <c r="C447" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="D447" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E447" s="2">
+        <v>20</v>
+      </c>
+      <c r="F447" s="1" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A448" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B448" s="13">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C448" s="4" t="s">
+        <v>974</v>
+      </c>
+      <c r="D448" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E448" s="2">
+        <v>30</v>
+      </c>
+      <c r="F448" s="1" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A449" s="5"/>
+      <c r="B449" s="13"/>
+      <c r="C449" s="4"/>
+      <c r="D449" s="2"/>
+      <c r="E449" s="2"/>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A450" s="5"/>
+      <c r="B450" s="13"/>
+      <c r="C450" s="4"/>
+      <c r="D450" s="2"/>
+      <c r="E450" s="2"/>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A451" s="5"/>
+      <c r="B451" s="13"/>
+      <c r="C451" s="4"/>
+      <c r="D451" s="2"/>
+      <c r="E451" s="2"/>
+    </row>
+    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A452" s="10"/>
       <c r="B452" s="10"/>
-    </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D452" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E452" s="3">
+        <f>SUM(E2:E448)</f>
+        <v>39970</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A453" s="10"/>
       <c r="B453" s="10"/>
-    </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D453" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E453" s="3">
+        <f>E452 / 60</f>
+        <v>666.16666666666663</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A454" s="10"/>
       <c r="B454" s="10"/>
     </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A455" s="10"/>
       <c r="B455" s="10"/>
     </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A456" s="10"/>
       <c r="B456" s="10"/>
     </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A457" s="10"/>
       <c r="B457" s="10"/>
     </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A458" s="10"/>
       <c r="B458" s="10"/>
     </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A459" s="10"/>
       <c r="B459" s="10"/>
     </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A460" s="10"/>
       <c r="B460" s="10"/>
     </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A461" s="10"/>
       <c r="B461" s="10"/>
     </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A462" s="10"/>
       <c r="B462" s="10"/>
     </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A463" s="10"/>
       <c r="B463" s="10"/>
     </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A464" s="10"/>
       <c r="B464" s="10"/>
     </row>
@@ -12883,6 +13387,98 @@
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A685" s="10"/>
       <c r="B685" s="10"/>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686" s="10"/>
+      <c r="B686" s="10"/>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687" s="10"/>
+      <c r="B687" s="10"/>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688" s="10"/>
+      <c r="B688" s="10"/>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A689" s="10"/>
+      <c r="B689" s="10"/>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A690" s="10"/>
+      <c r="B690" s="10"/>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A691" s="10"/>
+      <c r="B691" s="10"/>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A692" s="10"/>
+      <c r="B692" s="10"/>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A693" s="10"/>
+      <c r="B693" s="10"/>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A694" s="10"/>
+      <c r="B694" s="10"/>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A695" s="10"/>
+      <c r="B695" s="10"/>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A696" s="10"/>
+      <c r="B696" s="10"/>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A697" s="10"/>
+      <c r="B697" s="10"/>
+    </row>
+    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A698" s="10"/>
+      <c r="B698" s="10"/>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A699" s="10"/>
+      <c r="B699" s="10"/>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A700" s="10"/>
+      <c r="B700" s="10"/>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A701" s="10"/>
+      <c r="B701" s="10"/>
+    </row>
+    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A702" s="10"/>
+      <c r="B702" s="10"/>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A703" s="10"/>
+      <c r="B703" s="10"/>
+    </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A704" s="10"/>
+      <c r="B704" s="10"/>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A705" s="10"/>
+      <c r="B705" s="10"/>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A706" s="10"/>
+      <c r="B706" s="10"/>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A707" s="10"/>
+      <c r="B707" s="10"/>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A708" s="10"/>
+      <c r="B708" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>